<commit_message>
updated for June sales
</commit_message>
<xml_diff>
--- a/src/customers.xlsx
+++ b/src/customers.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J700"/>
+  <dimension ref="A1:J692"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -22956,22 +22956,22 @@
         </is>
       </c>
       <c r="C595">
-        <v>2292448</v>
+        <v>1618729</v>
       </c>
       <c r="D595">
-        <v>1262305.74</v>
+        <v>588587.16</v>
       </c>
       <c r="E595">
-        <v>2705090.04</v>
+        <v>1910101.62</v>
       </c>
       <c r="F595">
-        <v>322.88</v>
+        <v>227.99</v>
       </c>
       <c r="G595">
-        <v>7099.999999999999</v>
+        <v>7100</v>
       </c>
       <c r="H595">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I595" t="inlineStr">
         <is>
@@ -22994,22 +22994,22 @@
         </is>
       </c>
       <c r="C596">
-        <v>1947876</v>
+        <v>1392132</v>
       </c>
       <c r="D596">
-        <v>1206971.16</v>
+        <v>353448.48</v>
       </c>
       <c r="E596">
-        <v>2298493.44</v>
+        <v>1642715.52</v>
       </c>
       <c r="F596">
-        <v>231.89</v>
+        <v>165.73</v>
       </c>
       <c r="G596">
         <v>8400</v>
       </c>
       <c r="H596">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I596" t="inlineStr">
         <is>
@@ -23023,35 +23023,35 @@
     <row r="597">
       <c r="A597" t="inlineStr">
         <is>
-          <t>Adishakti Smelters Private Limited</t>
+          <t>Prakash Sponge Iron &amp; Power Pvt Ltd</t>
         </is>
       </c>
       <c r="B597" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C597">
-        <v>568997.5</v>
+        <v>693068</v>
       </c>
       <c r="D597">
-        <v>76816.24000000001</v>
+        <v>76749.12</v>
       </c>
       <c r="E597">
-        <v>620210</v>
+        <v>817819.8200000001</v>
       </c>
       <c r="F597">
-        <v>144.05</v>
+        <v>102.77</v>
       </c>
       <c r="G597">
-        <v>3950</v>
+        <v>6743.874671596769</v>
       </c>
       <c r="H597">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I597" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Shresth Maheshwari</t>
         </is>
       </c>
       <c r="J597" s="2">
@@ -23061,7 +23061,7 @@
     <row r="598">
       <c r="A598" t="inlineStr">
         <is>
-          <t>Suryadev Alloys &amp; Power Pvt Ltd</t>
+          <t>Suryadev Alloys &amp; Power Pvt Ltd Quartztech</t>
         </is>
       </c>
       <c r="B598" t="inlineStr">
@@ -23070,26 +23070,26 @@
         </is>
       </c>
       <c r="C598">
-        <v>946275</v>
+        <v>488628</v>
       </c>
       <c r="D598">
-        <v>537697</v>
+        <v>87953.04000000001</v>
       </c>
       <c r="E598">
-        <v>1116605</v>
+        <v>576581</v>
       </c>
       <c r="F598">
-        <v>126.17</v>
+        <v>77.56</v>
       </c>
       <c r="G598">
-        <v>7500.000000000001</v>
+        <v>6300</v>
       </c>
       <c r="H598">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I598" t="inlineStr">
         <is>
-          <t>Abhijit Maloo</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J598" s="2">
@@ -23099,31 +23099,31 @@
     <row r="599">
       <c r="A599" t="inlineStr">
         <is>
-          <t>Mahalakshmi Profiles Pvt Ltd</t>
+          <t>Adishakti Smelters Private Limited</t>
         </is>
       </c>
       <c r="B599" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C599">
-        <v>885271</v>
+        <v>284518.5</v>
       </c>
       <c r="D599">
-        <v>704193.86</v>
+        <v>51213.36</v>
       </c>
       <c r="E599">
-        <v>1044619.78</v>
+        <v>335731</v>
       </c>
       <c r="F599">
-        <v>121.27</v>
+        <v>72.03</v>
       </c>
       <c r="G599">
-        <v>7299.999999999999</v>
+        <v>3950</v>
       </c>
       <c r="H599">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I599" t="inlineStr">
         <is>
@@ -23137,7 +23137,7 @@
     <row r="600">
       <c r="A600" t="inlineStr">
         <is>
-          <t>Prakash Sponge Iron &amp; Power Pvt Ltd</t>
+          <t>A One Steel &amp; Alloys Pvt Ltd.(A One Steel (GBD))</t>
         </is>
       </c>
       <c r="B600" t="inlineStr">
@@ -23146,26 +23146,26 @@
         </is>
       </c>
       <c r="C600">
-        <v>741228</v>
+        <v>518419.5</v>
       </c>
       <c r="D600">
-        <v>474543.52</v>
+        <v>0</v>
       </c>
       <c r="E600">
-        <v>874648.48</v>
+        <v>611734.6799999999</v>
       </c>
       <c r="F600">
-        <v>97.53</v>
+        <v>65.21000000000001</v>
       </c>
       <c r="G600">
-        <v>7600.000000000001</v>
+        <v>7949.999999999999</v>
       </c>
       <c r="H600">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I600" t="inlineStr">
         <is>
-          <t>Shresth Maheshwari</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J600" s="2">
@@ -23175,35 +23175,35 @@
     <row r="601">
       <c r="A601" t="inlineStr">
         <is>
-          <t>Meenakshi Udyog India Pvt Ltd.</t>
+          <t>Mahrishi Alloys Pvt. Ltd.</t>
         </is>
       </c>
       <c r="B601" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C601">
-        <v>708474</v>
+        <v>201955</v>
       </c>
       <c r="D601">
-        <v>516593.64</v>
+        <v>15689.7</v>
       </c>
       <c r="E601">
-        <v>835999.36</v>
+        <v>238307.2</v>
       </c>
       <c r="F601">
-        <v>90.83</v>
+        <v>62.14</v>
       </c>
       <c r="G601">
-        <v>7799.999999999999</v>
+        <v>3250</v>
       </c>
       <c r="H601">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I601" t="inlineStr">
         <is>
-          <t>Abhijit Maloo</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J601" s="2">
@@ -23213,31 +23213,31 @@
     <row r="602">
       <c r="A602" t="inlineStr">
         <is>
-          <t>A One Ispat Private Ltd</t>
+          <t>Mahalakshmi Profiles Pvt Ltd</t>
         </is>
       </c>
       <c r="B602" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C602">
-        <v>661072</v>
+        <v>441723</v>
       </c>
       <c r="D602">
-        <v>95430.34</v>
+        <v>260646.5</v>
       </c>
       <c r="E602">
-        <v>732940</v>
+        <v>521233.14</v>
       </c>
       <c r="F602">
-        <v>83.68000000000001</v>
+        <v>60.51000000000001</v>
       </c>
       <c r="G602">
-        <v>7900</v>
+        <v>7299.999999999999</v>
       </c>
       <c r="H602">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I602" t="inlineStr">
         <is>
@@ -23251,35 +23251,35 @@
     <row r="603">
       <c r="A603" t="inlineStr">
         <is>
-          <t>Suryadev Alloys &amp; Power Pvt Ltd Quartztech</t>
+          <t>Meenakshi Udyog India Pvt Ltd.</t>
         </is>
       </c>
       <c r="B603" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C603">
-        <v>488628</v>
+        <v>471822</v>
       </c>
       <c r="D603">
-        <v>87953.04000000001</v>
+        <v>279942</v>
       </c>
       <c r="E603">
-        <v>576581</v>
+        <v>556750</v>
       </c>
       <c r="F603">
-        <v>77.56</v>
+        <v>60.48999999999999</v>
       </c>
       <c r="G603">
-        <v>6300</v>
+        <v>7800.000000000001</v>
       </c>
       <c r="H603">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I603" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Abhijit Maloo</t>
         </is>
       </c>
       <c r="J603" s="2">
@@ -23289,35 +23289,35 @@
     <row r="604">
       <c r="A604" t="inlineStr">
         <is>
-          <t>A One Steel &amp; Alloys Pvt Ltd.</t>
+          <t>Suryadev Alloys &amp; Power Pvt Ltd</t>
         </is>
       </c>
       <c r="B604" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C604">
-        <v>548311.5</v>
+        <v>449025</v>
       </c>
       <c r="D604">
-        <v>420148.28</v>
+        <v>40446</v>
       </c>
       <c r="E604">
-        <v>647006.6799999999</v>
+        <v>529850</v>
       </c>
       <c r="F604">
-        <v>68.97</v>
+        <v>59.87</v>
       </c>
       <c r="G604">
-        <v>7949.999999999999</v>
+        <v>7500</v>
       </c>
       <c r="H604">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I604" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Abhijit Maloo</t>
         </is>
       </c>
       <c r="J604" s="2">
@@ -23327,35 +23327,35 @@
     <row r="605">
       <c r="A605" t="inlineStr">
         <is>
-          <t>Prakash Sponge Iron &amp; Power Pvt Ltd</t>
+          <t>A One Ispat Private Ltd</t>
         </is>
       </c>
       <c r="B605" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C605">
-        <v>426384</v>
+        <v>399266</v>
       </c>
       <c r="D605">
-        <v>76749.12</v>
+        <v>71867.88</v>
       </c>
       <c r="E605">
-        <v>503132.82</v>
+        <v>471134</v>
       </c>
       <c r="F605">
-        <v>67.67999999999999</v>
+        <v>50.54000000000001</v>
       </c>
       <c r="G605">
-        <v>6300.000000000001</v>
+        <v>7899.999999999999</v>
       </c>
       <c r="H605">
         <v>2</v>
       </c>
       <c r="I605" t="inlineStr">
         <is>
-          <t>Shresth Maheshwari</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J605" s="2">
@@ -23365,31 +23365,31 @@
     <row r="606">
       <c r="A606" t="inlineStr">
         <is>
-          <t>Sri Navdurga Billets Pvt Ltd</t>
+          <t>Ardex Endura (India) Private Ltd Quartztech</t>
         </is>
       </c>
       <c r="B606" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Quartz Powder</t>
         </is>
       </c>
       <c r="C606">
-        <v>476106</v>
+        <v>126507.2</v>
       </c>
       <c r="D606">
-        <v>297364</v>
+        <v>6325.360000000001</v>
       </c>
       <c r="E606">
-        <v>561805.04</v>
+        <v>132832.64</v>
       </c>
       <c r="F606">
-        <v>65.22</v>
+        <v>46.51000000000001</v>
       </c>
       <c r="G606">
-        <v>7300.000000000001</v>
+        <v>2720</v>
       </c>
       <c r="H606">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I606" t="inlineStr">
         <is>
@@ -23403,35 +23403,35 @@
     <row r="607">
       <c r="A607" t="inlineStr">
         <is>
-          <t>Orange Fox Steel Pvt Ltd</t>
+          <t>Kanishk Steel Industries Ltd</t>
         </is>
       </c>
       <c r="B607" t="inlineStr">
         <is>
-          <t>Nali Top</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C607">
-        <v>218046</v>
+        <v>288864</v>
       </c>
       <c r="D607">
-        <v>160445.72</v>
+        <v>0</v>
       </c>
       <c r="E607">
-        <v>228948.3</v>
+        <v>340860</v>
       </c>
       <c r="F607">
-        <v>63.19</v>
+        <v>40.12</v>
       </c>
       <c r="G607">
-        <v>3450.640924196867</v>
+        <v>7200.000000000001</v>
       </c>
       <c r="H607">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I607" t="inlineStr">
         <is>
-          <t>Sunil Rathi</t>
+          <t>Abhijit Maloo</t>
         </is>
       </c>
       <c r="J607" s="2">
@@ -23441,31 +23441,31 @@
     <row r="608">
       <c r="A608" t="inlineStr">
         <is>
-          <t>Mahrishi Alloys Pvt. Ltd.</t>
+          <t>A One Steel &amp; Alloys Pvt Ltd.</t>
         </is>
       </c>
       <c r="B608" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C608">
-        <v>201955</v>
+        <v>307585.5</v>
       </c>
       <c r="D608">
-        <v>15689.7</v>
+        <v>179421.96</v>
       </c>
       <c r="E608">
-        <v>238307.2</v>
+        <v>362950</v>
       </c>
       <c r="F608">
-        <v>62.14</v>
+        <v>38.69</v>
       </c>
       <c r="G608">
-        <v>3250</v>
+        <v>7950.000000000001</v>
       </c>
       <c r="H608">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I608" t="inlineStr">
         <is>
@@ -23479,7 +23479,7 @@
     <row r="609">
       <c r="A609" t="inlineStr">
         <is>
-          <t>Pushpit Steels Private Limited</t>
+          <t>Orange Fox Steel Pvt Ltd</t>
         </is>
       </c>
       <c r="B609" t="inlineStr">
@@ -23488,26 +23488,26 @@
         </is>
       </c>
       <c r="C609">
-        <v>382292</v>
+        <v>226137</v>
       </c>
       <c r="D609">
-        <v>51330.14</v>
+        <v>40704.66</v>
       </c>
       <c r="E609">
-        <v>416140.28</v>
+        <v>266842</v>
       </c>
       <c r="F609">
-        <v>61.66</v>
+        <v>35.06</v>
       </c>
       <c r="G609">
-        <v>6200</v>
+        <v>6450</v>
       </c>
       <c r="H609">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I609" t="inlineStr">
         <is>
-          <t>Abhijit Maloo</t>
+          <t>Sunil Rathi</t>
         </is>
       </c>
       <c r="J609" s="2">
@@ -23517,31 +23517,31 @@
     <row r="610">
       <c r="A610" t="inlineStr">
         <is>
-          <t>S K STEEL TECH PRIVATE LIMITED_x000D_</t>
+          <t>Prakash Sponge Iron &amp; Power Pvt Ltd</t>
         </is>
       </c>
       <c r="B610" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C610">
-        <v>386304</v>
+        <v>238108</v>
       </c>
       <c r="D610">
-        <v>227919</v>
+        <v>238108</v>
       </c>
       <c r="E610">
-        <v>455838.36</v>
+        <v>280967</v>
       </c>
       <c r="F610">
-        <v>60.36</v>
+        <v>31.33</v>
       </c>
       <c r="G610">
-        <v>6400</v>
+        <v>7600</v>
       </c>
       <c r="H610">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I610" t="inlineStr">
         <is>
@@ -23555,35 +23555,35 @@
     <row r="611">
       <c r="A611" t="inlineStr">
         <is>
-          <t>JEPPIAAR FURNACE AND STEELS PVT.LTD</t>
+          <t>ILC IRON &amp; STEEL PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="B611" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C611">
-        <v>553196</v>
+        <v>192944</v>
       </c>
       <c r="D611">
-        <v>553196.28</v>
+        <v>34729.92</v>
       </c>
       <c r="E611">
-        <v>652771.72</v>
+        <v>227674</v>
       </c>
       <c r="F611">
-        <v>60.13</v>
+        <v>31.12</v>
       </c>
       <c r="G611">
-        <v>9200</v>
+        <v>6200</v>
       </c>
       <c r="H611">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I611" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Shresth Maheshwari</t>
         </is>
       </c>
       <c r="J611" s="2">
@@ -23593,7 +23593,7 @@
     <row r="612">
       <c r="A612" t="inlineStr">
         <is>
-          <t>M S METALS AND STEELS PVT LTD (ANCHEPALYA)</t>
+          <t>A One Steels And Alloys Pvt Ltd</t>
         </is>
       </c>
       <c r="B612" t="inlineStr">
@@ -23602,22 +23602,22 @@
         </is>
       </c>
       <c r="C612">
-        <v>473760</v>
+        <v>264708</v>
       </c>
       <c r="D612">
-        <v>473760.4</v>
+        <v>264708</v>
       </c>
       <c r="E612">
-        <v>559036.6</v>
+        <v>312355</v>
       </c>
       <c r="F612">
-        <v>59.22</v>
+        <v>30.78</v>
       </c>
       <c r="G612">
-        <v>7999.999999999999</v>
+        <v>8600</v>
       </c>
       <c r="H612">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I612" t="inlineStr">
         <is>
@@ -23631,31 +23631,31 @@
     <row r="613">
       <c r="A613" t="inlineStr">
         <is>
-          <t>Ardex Endura (India) Private Ltd Quartztech</t>
+          <t>Sugna Sponge &amp; Power Pvt Ltd</t>
         </is>
       </c>
       <c r="B613" t="inlineStr">
         <is>
-          <t>Quartz Powder</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C613">
-        <v>126507.2</v>
+        <v>98496</v>
       </c>
       <c r="D613">
-        <v>6325.360000000001</v>
+        <v>17729.28</v>
       </c>
       <c r="E613">
-        <v>132832.64</v>
+        <v>116225.28</v>
       </c>
       <c r="F613">
-        <v>46.51000000000001</v>
+        <v>30.78</v>
       </c>
       <c r="G613">
-        <v>2720</v>
+        <v>3200</v>
       </c>
       <c r="H613">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I613" t="inlineStr">
         <is>
@@ -23669,7 +23669,7 @@
     <row r="614">
       <c r="A614" t="inlineStr">
         <is>
-          <t>Kanishk Steel Industries Ltd</t>
+          <t>GOVAAN STEELS PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="B614" t="inlineStr">
@@ -23678,26 +23678,26 @@
         </is>
       </c>
       <c r="C614">
-        <v>288864</v>
+        <v>194240</v>
       </c>
       <c r="D614">
         <v>0</v>
       </c>
       <c r="E614">
-        <v>340860</v>
+        <v>229203.2</v>
       </c>
       <c r="F614">
-        <v>40.12</v>
+        <v>30.35</v>
       </c>
       <c r="G614">
-        <v>7200.000000000001</v>
+        <v>6400</v>
       </c>
       <c r="H614">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I614" t="inlineStr">
         <is>
-          <t>Abhijit Maloo</t>
+          <t>Vishnu Kankani</t>
         </is>
       </c>
       <c r="J614" s="2">
@@ -23716,22 +23716,22 @@
         </is>
       </c>
       <c r="C615">
-        <v>57784</v>
+        <v>47011.5</v>
       </c>
       <c r="D615">
-        <v>30093.485</v>
+        <v>29124.32</v>
       </c>
       <c r="E615">
-        <v>68184.63</v>
+        <v>55473.08</v>
       </c>
       <c r="F615">
-        <v>37.28</v>
+        <v>30.33</v>
       </c>
       <c r="G615">
         <v>1550</v>
       </c>
       <c r="H615">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I615" t="inlineStr">
         <is>
@@ -23745,7 +23745,7 @@
     <row r="616">
       <c r="A616" t="inlineStr">
         <is>
-          <t>Orange Fox Steel Pvt Ltd</t>
+          <t>Pushpit Steels Private Limited</t>
         </is>
       </c>
       <c r="B616" t="inlineStr">
@@ -23754,26 +23754,26 @@
         </is>
       </c>
       <c r="C616">
-        <v>226137</v>
+        <v>188046</v>
       </c>
       <c r="D616">
-        <v>40704.66</v>
+        <v>33848.28</v>
       </c>
       <c r="E616">
-        <v>266842</v>
+        <v>221894.28</v>
       </c>
       <c r="F616">
-        <v>35.06</v>
+        <v>30.33</v>
       </c>
       <c r="G616">
-        <v>6450</v>
+        <v>6200</v>
       </c>
       <c r="H616">
         <v>1</v>
       </c>
       <c r="I616" t="inlineStr">
         <is>
-          <t>Sunil Rathi</t>
+          <t>Abhijit Maloo</t>
         </is>
       </c>
       <c r="J616" s="2">
@@ -23783,28 +23783,28 @@
     <row r="617">
       <c r="A617" t="inlineStr">
         <is>
-          <t>A One Steel &amp; Alloys Pvt Ltd.(A One Steel (GBD))</t>
+          <t>M S METALS AND STEELS PVT LTD (ANCHEPALYA)</t>
         </is>
       </c>
       <c r="B617" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C617">
-        <v>277693.5</v>
+        <v>204322.5</v>
       </c>
       <c r="D617">
-        <v>0</v>
+        <v>36778.05</v>
       </c>
       <c r="E617">
-        <v>327678</v>
+        <v>241101</v>
       </c>
       <c r="F617">
-        <v>34.93</v>
+        <v>30.27</v>
       </c>
       <c r="G617">
-        <v>7950</v>
+        <v>6750</v>
       </c>
       <c r="H617">
         <v>1</v>
@@ -23821,31 +23821,31 @@
     <row r="618">
       <c r="A618" t="inlineStr">
         <is>
-          <t>Shri Tirupati Steel Cast Ltd</t>
+          <t>A One Steels And Alloys Pvt Ltd(A One Bellary)</t>
         </is>
       </c>
       <c r="B618" t="inlineStr">
         <is>
-          <t>Nali Top</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C618">
-        <v>110912</v>
+        <v>260064</v>
       </c>
       <c r="D618">
-        <v>16396.2</v>
+        <v>0</v>
       </c>
       <c r="E618">
-        <v>123740</v>
+        <v>306876</v>
       </c>
       <c r="F618">
-        <v>34.66</v>
+        <v>30.24</v>
       </c>
       <c r="G618">
-        <v>3200</v>
+        <v>8600</v>
       </c>
       <c r="H618">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I618" t="inlineStr">
         <is>
@@ -23859,7 +23859,7 @@
     <row r="619">
       <c r="A619" t="inlineStr">
         <is>
-          <t>A One Steels And Alloys Pvt Ltd</t>
+          <t>S K STEEL TECH PRIVATE LIMITED_x000D_</t>
         </is>
       </c>
       <c r="B619" t="inlineStr">
@@ -23868,26 +23868,26 @@
         </is>
       </c>
       <c r="C619">
-        <v>221357.5</v>
+        <v>193152</v>
       </c>
       <c r="D619">
-        <v>221357.65</v>
+        <v>34767.36</v>
       </c>
       <c r="E619">
-        <v>261201.85</v>
+        <v>227919</v>
       </c>
       <c r="F619">
-        <v>31.85</v>
+        <v>30.18</v>
       </c>
       <c r="G619">
-        <v>6950</v>
+        <v>6400</v>
       </c>
       <c r="H619">
         <v>2</v>
       </c>
       <c r="I619" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Shresth Maheshwari</t>
         </is>
       </c>
       <c r="J619" s="2">
@@ -23897,7 +23897,7 @@
     <row r="620">
       <c r="A620" t="inlineStr">
         <is>
-          <t>ILC IRON &amp; STEEL PRIVATE LIMITED</t>
+          <t>SHRADDHA ISPAT-MELTING DIVISION</t>
         </is>
       </c>
       <c r="B620" t="inlineStr">
@@ -23906,19 +23906,19 @@
         </is>
       </c>
       <c r="C620">
-        <v>192944</v>
+        <v>192768</v>
       </c>
       <c r="D620">
-        <v>34729.92</v>
+        <v>0</v>
       </c>
       <c r="E620">
-        <v>227674</v>
+        <v>227466.24</v>
       </c>
       <c r="F620">
-        <v>31.12</v>
+        <v>30.12</v>
       </c>
       <c r="G620">
-        <v>6200</v>
+        <v>6400</v>
       </c>
       <c r="H620">
         <v>1</v>
@@ -23935,35 +23935,35 @@
     <row r="621">
       <c r="A621" t="inlineStr">
         <is>
-          <t>Sri Vigneshwara Steels (p) Ltd</t>
+          <t>JEPPIAAR FURNACE AND STEELS PVT.LTD</t>
         </is>
       </c>
       <c r="B621" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C621">
-        <v>193977</v>
+        <v>276092</v>
       </c>
       <c r="D621">
-        <v>193977.14</v>
+        <v>276092</v>
       </c>
       <c r="E621">
-        <v>228892.86</v>
+        <v>325789</v>
       </c>
       <c r="F621">
-        <v>30.79</v>
+        <v>30.01</v>
       </c>
       <c r="G621">
-        <v>6300</v>
+        <v>9200</v>
       </c>
       <c r="H621">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I621" t="inlineStr">
         <is>
-          <t>Vishnu Kankani</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J621" s="2">
@@ -23973,31 +23973,31 @@
     <row r="622">
       <c r="A622" t="inlineStr">
         <is>
-          <t>A One Steels And Alloys Pvt Ltd</t>
+          <t>AMBA FRP PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="B622" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Quartz Grain</t>
         </is>
       </c>
       <c r="C622">
-        <v>264708</v>
+        <v>180000</v>
       </c>
       <c r="D622">
-        <v>264708</v>
+        <v>9000</v>
       </c>
       <c r="E622">
-        <v>312355</v>
+        <v>189000</v>
       </c>
       <c r="F622">
-        <v>30.78</v>
+        <v>30</v>
       </c>
       <c r="G622">
-        <v>8600</v>
+        <v>6000</v>
       </c>
       <c r="H622">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I622" t="inlineStr">
         <is>
@@ -24011,31 +24011,31 @@
     <row r="623">
       <c r="A623" t="inlineStr">
         <is>
-          <t>Sugna Sponge &amp; Power Pvt Ltd</t>
+          <t>Sri Navdurga Billets Pvt Ltd</t>
         </is>
       </c>
       <c r="B623" t="inlineStr">
         <is>
-          <t>Nali Top</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C623">
-        <v>98496</v>
+        <v>217978</v>
       </c>
       <c r="D623">
-        <v>17729.28</v>
+        <v>39236.04</v>
       </c>
       <c r="E623">
-        <v>116225.28</v>
+        <v>257214</v>
       </c>
       <c r="F623">
-        <v>30.78</v>
+        <v>29.86</v>
       </c>
       <c r="G623">
-        <v>3200</v>
+        <v>7300</v>
       </c>
       <c r="H623">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I623" t="inlineStr">
         <is>
@@ -24049,7 +24049,7 @@
     <row r="624">
       <c r="A624" t="inlineStr">
         <is>
-          <t>Sree Rengaraj Ispat Industries (P) Ltd</t>
+          <t>Jai Hind Wire Rod Mills Private Limited</t>
         </is>
       </c>
       <c r="B624" t="inlineStr">
@@ -24058,22 +24058,22 @@
         </is>
       </c>
       <c r="C624">
-        <v>192465</v>
+        <v>226328</v>
       </c>
       <c r="D624">
-        <v>192465.3</v>
+        <v>226328</v>
       </c>
       <c r="E624">
-        <v>227108.7</v>
+        <v>267067</v>
       </c>
       <c r="F624">
-        <v>30.55</v>
+        <v>29.78</v>
       </c>
       <c r="G624">
-        <v>6300</v>
+        <v>7600</v>
       </c>
       <c r="H624">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I624" t="inlineStr">
         <is>
@@ -24087,7 +24087,7 @@
     <row r="625">
       <c r="A625" t="inlineStr">
         <is>
-          <t>GOVAAN STEELS PRIVATE LIMITED</t>
+          <t>Sri Vinayaga Alloys (P) Ltd</t>
         </is>
       </c>
       <c r="B625" t="inlineStr">
@@ -24096,19 +24096,19 @@
         </is>
       </c>
       <c r="C625">
-        <v>194240</v>
+        <v>187047</v>
       </c>
       <c r="D625">
-        <v>0</v>
+        <v>33668.46</v>
       </c>
       <c r="E625">
-        <v>229203.2</v>
+        <v>220715</v>
       </c>
       <c r="F625">
-        <v>30.35</v>
+        <v>29.69</v>
       </c>
       <c r="G625">
-        <v>6400</v>
+        <v>6300</v>
       </c>
       <c r="H625">
         <v>1</v>
@@ -24130,23 +24130,23 @@
       </c>
       <c r="B626" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C626">
-        <v>204322.5</v>
+        <v>234240</v>
       </c>
       <c r="D626">
-        <v>36778.05</v>
+        <v>234240</v>
       </c>
       <c r="E626">
-        <v>241101</v>
+        <v>276403</v>
       </c>
       <c r="F626">
-        <v>30.27</v>
+        <v>29.28</v>
       </c>
       <c r="G626">
-        <v>6750</v>
+        <v>8000</v>
       </c>
       <c r="H626">
         <v>1</v>
@@ -24163,28 +24163,28 @@
     <row r="627">
       <c r="A627" t="inlineStr">
         <is>
-          <t>A One Steels And Alloys Pvt Ltd(A One Bellary)</t>
+          <t>Sree  Rengaraaj Steel &amp; Alloys (P) Limited</t>
         </is>
       </c>
       <c r="B627" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Ordinary Ramming Mass</t>
         </is>
       </c>
       <c r="C627">
-        <v>260064</v>
+        <v>111936</v>
       </c>
       <c r="D627">
-        <v>0</v>
+        <v>20148.48</v>
       </c>
       <c r="E627">
-        <v>306876</v>
+        <v>132084</v>
       </c>
       <c r="F627">
-        <v>30.24</v>
+        <v>25.44</v>
       </c>
       <c r="G627">
-        <v>8600</v>
+        <v>4400</v>
       </c>
       <c r="H627">
         <v>1</v>
@@ -24201,35 +24201,35 @@
     <row r="628">
       <c r="A628" t="inlineStr">
         <is>
-          <t>Noble Tech Industries Pvt Ltd</t>
+          <t>Tulsyan NEC Limited</t>
         </is>
       </c>
       <c r="B628" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C628">
-        <v>271080</v>
+        <v>191770</v>
       </c>
       <c r="D628">
-        <v>271079.6</v>
+        <v>34518.6</v>
       </c>
       <c r="E628">
-        <v>319874.4</v>
+        <v>226289</v>
       </c>
       <c r="F628">
-        <v>30.12</v>
+        <v>25.4</v>
       </c>
       <c r="G628">
-        <v>9000</v>
+        <v>7550</v>
       </c>
       <c r="H628">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I628" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Abhijit Maloo</t>
         </is>
       </c>
       <c r="J628" s="2">
@@ -24239,7 +24239,7 @@
     <row r="629">
       <c r="A629" t="inlineStr">
         <is>
-          <t>SHRADDHA ISPAT-MELTING DIVISION</t>
+          <t>Pattambi Brothers</t>
         </is>
       </c>
       <c r="B629" t="inlineStr">
@@ -24248,26 +24248,26 @@
         </is>
       </c>
       <c r="C629">
-        <v>192768</v>
+        <v>159138</v>
       </c>
       <c r="D629">
-        <v>192767.76</v>
+        <v>0</v>
       </c>
       <c r="E629">
-        <v>202406.4</v>
+        <v>187782.84</v>
       </c>
       <c r="F629">
-        <v>30.12</v>
+        <v>25.26</v>
       </c>
       <c r="G629">
-        <v>6400</v>
+        <v>6300</v>
       </c>
       <c r="H629">
         <v>1</v>
       </c>
       <c r="I629" t="inlineStr">
         <is>
-          <t>Sunil Rathi</t>
+          <t>Vishnu Kankani</t>
         </is>
       </c>
       <c r="J629" s="2">
@@ -24277,35 +24277,35 @@
     <row r="630">
       <c r="A630" t="inlineStr">
         <is>
-          <t>AMBA FRP PRIVATE LIMITED</t>
+          <t>Prakash Ferrous Industries Pvt Ltd</t>
         </is>
       </c>
       <c r="B630" t="inlineStr">
         <is>
-          <t>Quartz Grain</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C630">
-        <v>180000</v>
+        <v>176050</v>
       </c>
       <c r="D630">
-        <v>9000</v>
+        <v>31689</v>
       </c>
       <c r="E630">
-        <v>189000</v>
+        <v>207739</v>
       </c>
       <c r="F630">
-        <v>30</v>
+        <v>25.15</v>
       </c>
       <c r="G630">
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="H630">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I630" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Abhijit Maloo</t>
         </is>
       </c>
       <c r="J630" s="2">
@@ -24315,35 +24315,35 @@
     <row r="631">
       <c r="A631" t="inlineStr">
         <is>
-          <t>Jai Hind Wire Rod Mills Private Limited</t>
+          <t>RELIANCE CONCAST SOLUTIONS</t>
         </is>
       </c>
       <c r="B631" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Quartz Powder</t>
         </is>
       </c>
       <c r="C631">
-        <v>226328</v>
+        <v>65720</v>
       </c>
       <c r="D631">
-        <v>226328</v>
+        <v>0</v>
       </c>
       <c r="E631">
-        <v>267067</v>
+        <v>69006</v>
       </c>
       <c r="F631">
-        <v>29.78</v>
+        <v>24.8</v>
       </c>
       <c r="G631">
-        <v>7600</v>
+        <v>2650</v>
       </c>
       <c r="H631">
         <v>1</v>
       </c>
       <c r="I631" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Shresth Maheshwari</t>
         </is>
       </c>
       <c r="J631" s="2">
@@ -24353,35 +24353,35 @@
     <row r="632">
       <c r="A632" t="inlineStr">
         <is>
-          <t>Sri Vinayaga Alloys (P) Ltd</t>
+          <t>Shri Tirupati Steel Cast Ltd</t>
         </is>
       </c>
       <c r="B632" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C632">
-        <v>187047</v>
+        <v>71264</v>
       </c>
       <c r="D632">
-        <v>33668.46</v>
+        <v>12827.52</v>
       </c>
       <c r="E632">
-        <v>220715</v>
+        <v>84092</v>
       </c>
       <c r="F632">
-        <v>29.69</v>
+        <v>22.27</v>
       </c>
       <c r="G632">
-        <v>6300</v>
+        <v>3200</v>
       </c>
       <c r="H632">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I632" t="inlineStr">
         <is>
-          <t>Vishnu Kankani</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J632" s="2">
@@ -24391,7 +24391,7 @@
     <row r="633">
       <c r="A633" t="inlineStr">
         <is>
-          <t>Prime Gold International Limited</t>
+          <t>Meenakshi Steels</t>
         </is>
       </c>
       <c r="B633" t="inlineStr">
@@ -24400,26 +24400,26 @@
         </is>
       </c>
       <c r="C633">
-        <v>235840</v>
+        <v>129960</v>
       </c>
       <c r="D633">
-        <v>235839.8</v>
+        <v>0</v>
       </c>
       <c r="E633">
-        <v>278291.2</v>
+        <v>153352.8</v>
       </c>
       <c r="F633">
-        <v>29.48</v>
+        <v>21.66</v>
       </c>
       <c r="G633">
-        <v>8000</v>
+        <v>6000</v>
       </c>
       <c r="H633">
         <v>2</v>
       </c>
       <c r="I633" t="inlineStr">
         <is>
-          <t>Sharad Bhutra</t>
+          <t>Abhijit Maloo</t>
         </is>
       </c>
       <c r="J633" s="2">
@@ -24429,31 +24429,31 @@
     <row r="634">
       <c r="A634" t="inlineStr">
         <is>
-          <t>Sree  Rengaraaj Steel &amp; Alloys (P) Limited</t>
+          <t>Rama Hi Power Tech</t>
         </is>
       </c>
       <c r="B634" t="inlineStr">
         <is>
-          <t>Ordinary Ramming Mass</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C634">
-        <v>111936</v>
+        <v>148400</v>
       </c>
       <c r="D634">
-        <v>20148.48</v>
+        <v>87290</v>
       </c>
       <c r="E634">
-        <v>132084</v>
+        <v>175111.8</v>
       </c>
       <c r="F634">
-        <v>25.44</v>
+        <v>21.2</v>
       </c>
       <c r="G634">
-        <v>4400</v>
+        <v>6999.999999999999</v>
       </c>
       <c r="H634">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I634" t="inlineStr">
         <is>
@@ -24467,7 +24467,7 @@
     <row r="635">
       <c r="A635" t="inlineStr">
         <is>
-          <t>Tulsyan NEC Limited</t>
+          <t>PURVA STEEL PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="B635" t="inlineStr">
@@ -24476,26 +24476,26 @@
         </is>
       </c>
       <c r="C635">
-        <v>191770</v>
+        <v>135616</v>
       </c>
       <c r="D635">
-        <v>34518.6</v>
+        <v>18397.44</v>
       </c>
       <c r="E635">
-        <v>226289</v>
+        <v>160026.44</v>
       </c>
       <c r="F635">
-        <v>25.4</v>
+        <v>21.19</v>
       </c>
       <c r="G635">
-        <v>7550</v>
+        <v>6400</v>
       </c>
       <c r="H635">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I635" t="inlineStr">
         <is>
-          <t>Abhijit Maloo</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J635" s="2">
@@ -24505,7 +24505,7 @@
     <row r="636">
       <c r="A636" t="inlineStr">
         <is>
-          <t>Pattambi Brothers</t>
+          <t>Adishakti Smelters Private Limited</t>
         </is>
       </c>
       <c r="B636" t="inlineStr">
@@ -24514,26 +24514,26 @@
         </is>
       </c>
       <c r="C636">
-        <v>159138</v>
+        <v>64415</v>
       </c>
       <c r="D636">
-        <v>159138.16</v>
+        <v>11594.72</v>
       </c>
       <c r="E636">
-        <v>187782.84</v>
+        <v>76009</v>
       </c>
       <c r="F636">
-        <v>25.26</v>
+        <v>19.82</v>
       </c>
       <c r="G636">
-        <v>6300</v>
+        <v>3250</v>
       </c>
       <c r="H636">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I636" t="inlineStr">
         <is>
-          <t>Vishnu Kankani</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J636" s="2">
@@ -24543,28 +24543,28 @@
     <row r="637">
       <c r="A637" t="inlineStr">
         <is>
-          <t>Prakash Ferrous Industries Pvt Ltd</t>
+          <t>Meenakshi Steels</t>
         </is>
       </c>
       <c r="B637" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C637">
-        <v>176050</v>
+        <v>100932</v>
       </c>
       <c r="D637">
-        <v>31689</v>
+        <v>0</v>
       </c>
       <c r="E637">
-        <v>207739</v>
+        <v>119099.76</v>
       </c>
       <c r="F637">
-        <v>25.15</v>
+        <v>12.94</v>
       </c>
       <c r="G637">
-        <v>7000</v>
+        <v>7800</v>
       </c>
       <c r="H637">
         <v>1</v>
@@ -24581,35 +24581,35 @@
     <row r="638">
       <c r="A638" t="inlineStr">
         <is>
-          <t>RELIANCE CONCAST SOLUTIONS</t>
+          <t>PURVA STEEL PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="B638" t="inlineStr">
         <is>
-          <t>Quartz Powder</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C638">
-        <v>65720</v>
+        <v>34102</v>
       </c>
       <c r="D638">
-        <v>0</v>
+        <v>12151.8</v>
       </c>
       <c r="E638">
-        <v>69006</v>
+        <v>40240.36</v>
       </c>
       <c r="F638">
-        <v>24.8</v>
+        <v>10.03</v>
       </c>
       <c r="G638">
-        <v>2650</v>
+        <v>3400</v>
       </c>
       <c r="H638">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I638" t="inlineStr">
         <is>
-          <t>Shresth Maheshwari</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J638" s="2">
@@ -24619,28 +24619,28 @@
     <row r="639">
       <c r="A639" t="inlineStr">
         <is>
-          <t>Adishakti Smelters Private Limited</t>
+          <t>MEGA TMT AND STEEL INDUSTRIES PVT LTD</t>
         </is>
       </c>
       <c r="B639" t="inlineStr">
         <is>
-          <t>Nali Top</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C639">
-        <v>38608</v>
+        <v>64218</v>
       </c>
       <c r="D639">
-        <v>4601.84</v>
+        <v>11559.24</v>
       </c>
       <c r="E639">
-        <v>40863</v>
+        <v>75777</v>
       </c>
       <c r="F639">
-        <v>24.13</v>
+        <v>9.73</v>
       </c>
       <c r="G639">
-        <v>1600</v>
+        <v>6600</v>
       </c>
       <c r="H639">
         <v>3</v>
@@ -24657,35 +24657,35 @@
     <row r="640">
       <c r="A640" t="inlineStr">
         <is>
-          <t>Meenakshi Steels</t>
+          <t>Adishakti Smelters Private Limited</t>
         </is>
       </c>
       <c r="B640" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C640">
-        <v>129960</v>
+        <v>12528</v>
       </c>
       <c r="D640">
-        <v>0</v>
+        <v>2255.04</v>
       </c>
       <c r="E640">
-        <v>153352.8</v>
+        <v>14783</v>
       </c>
       <c r="F640">
-        <v>21.66</v>
+        <v>7.83</v>
       </c>
       <c r="G640">
-        <v>6000</v>
+        <v>1600</v>
       </c>
       <c r="H640">
         <v>2</v>
       </c>
       <c r="I640" t="inlineStr">
         <is>
-          <t>Abhijit Maloo</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J640" s="2">
@@ -24700,26 +24700,26 @@
       </c>
       <c r="B641" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C641">
-        <v>148400</v>
+        <v>15640</v>
       </c>
       <c r="D641">
-        <v>87290</v>
+        <v>13815</v>
       </c>
       <c r="E641">
-        <v>175111.8</v>
+        <v>18455.2</v>
       </c>
       <c r="F641">
-        <v>21.2</v>
+        <v>4.6</v>
       </c>
       <c r="G641">
-        <v>6999.999999999999</v>
+        <v>3400</v>
       </c>
       <c r="H641">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I641" t="inlineStr">
         <is>
@@ -24733,7 +24733,7 @@
     <row r="642">
       <c r="A642" t="inlineStr">
         <is>
-          <t>PURVA STEEL PRIVATE LIMITED</t>
+          <t>SAMKRG PISTONS AND RINGS LIMITED</t>
         </is>
       </c>
       <c r="B642" t="inlineStr">
@@ -24742,22 +24742,22 @@
         </is>
       </c>
       <c r="C642">
-        <v>135616</v>
+        <v>9920</v>
       </c>
       <c r="D642">
-        <v>18397.44</v>
+        <v>1785.6</v>
       </c>
       <c r="E642">
-        <v>160026.44</v>
+        <v>11706</v>
       </c>
       <c r="F642">
-        <v>21.19</v>
+        <v>1.24</v>
       </c>
       <c r="G642">
-        <v>6400</v>
+        <v>8000</v>
       </c>
       <c r="H642">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I642" t="inlineStr">
         <is>
@@ -24771,7 +24771,7 @@
     <row r="643">
       <c r="A643" t="inlineStr">
         <is>
-          <t>Mahrishi Alloys Pvt. Ltd.</t>
+          <t>Minera Steel &amp; Power Pvt Ltd</t>
         </is>
       </c>
       <c r="B643" t="inlineStr">
@@ -24780,36 +24780,36 @@
         </is>
       </c>
       <c r="C643">
-        <v>79760</v>
+        <v>2447424</v>
       </c>
       <c r="D643">
-        <v>7178.4</v>
+        <v>440536.32</v>
       </c>
       <c r="E643">
-        <v>94116.79999999999</v>
+        <v>2887959</v>
       </c>
       <c r="F643">
-        <v>19.94</v>
+        <v>291.36</v>
       </c>
       <c r="G643">
-        <v>4000</v>
+        <v>8400</v>
       </c>
       <c r="H643">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="I643" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Vishnu Kankani</t>
         </is>
       </c>
       <c r="J643" s="2">
-        <v>45047</v>
+        <v>45078</v>
       </c>
     </row>
     <row r="644">
       <c r="A644" t="inlineStr">
         <is>
-          <t>Adishakti Smelters Private Limited</t>
+          <t>BMM ISPAT LIMITED</t>
         </is>
       </c>
       <c r="B644" t="inlineStr">
@@ -24818,22 +24818,22 @@
         </is>
       </c>
       <c r="C644">
-        <v>64415</v>
+        <v>2051687</v>
       </c>
       <c r="D644">
-        <v>11594.72</v>
+        <v>369303.66</v>
       </c>
       <c r="E644">
-        <v>76009</v>
+        <v>2420991</v>
       </c>
       <c r="F644">
-        <v>19.82</v>
+        <v>288.97</v>
       </c>
       <c r="G644">
-        <v>3250</v>
+        <v>7100.000000000001</v>
       </c>
       <c r="H644">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I644" t="inlineStr">
         <is>
@@ -24841,37 +24841,37 @@
         </is>
       </c>
       <c r="J644" s="2">
-        <v>45047</v>
+        <v>45078</v>
       </c>
     </row>
     <row r="645">
       <c r="A645" t="inlineStr">
         <is>
-          <t>Meenakshi Steels</t>
+          <t>Suryadev Alloys &amp; Power Pvt Ltd</t>
         </is>
       </c>
       <c r="B645" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C645">
-        <v>100932</v>
+        <v>1389000</v>
       </c>
       <c r="D645">
-        <v>0</v>
+        <v>250020</v>
       </c>
       <c r="E645">
-        <v>119099.76</v>
+        <v>1639022</v>
       </c>
       <c r="F645">
-        <v>12.94</v>
+        <v>185.2</v>
       </c>
       <c r="G645">
-        <v>7800</v>
+        <v>7500</v>
       </c>
       <c r="H645">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I645" t="inlineStr">
         <is>
@@ -24879,51 +24879,51 @@
         </is>
       </c>
       <c r="J645" s="2">
-        <v>45047</v>
+        <v>45078</v>
       </c>
     </row>
     <row r="646">
       <c r="A646" t="inlineStr">
         <is>
-          <t>PURVA STEEL PRIVATE LIMITED</t>
+          <t>Pushpit Steels Private Limited</t>
         </is>
       </c>
       <c r="B646" t="inlineStr">
         <is>
-          <t>Nali Top</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C646">
-        <v>34102</v>
+        <v>1058402</v>
       </c>
       <c r="D646">
-        <v>12151.8</v>
+        <v>190512.36</v>
       </c>
       <c r="E646">
-        <v>40240.36</v>
+        <v>1248913</v>
       </c>
       <c r="F646">
-        <v>10.03</v>
+        <v>170.71</v>
       </c>
       <c r="G646">
-        <v>3400</v>
+        <v>6200</v>
       </c>
       <c r="H646">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I646" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Abhijit Maloo</t>
         </is>
       </c>
       <c r="J646" s="2">
-        <v>45047</v>
+        <v>45078</v>
       </c>
     </row>
     <row r="647">
       <c r="A647" t="inlineStr">
         <is>
-          <t>MEGA TMT AND STEEL INDUSTRIES PVT LTD</t>
+          <t>Suryadev Alloys &amp; Power Pvt Ltd Quartztech</t>
         </is>
       </c>
       <c r="B647" t="inlineStr">
@@ -24932,22 +24932,22 @@
         </is>
       </c>
       <c r="C647">
-        <v>64218</v>
+        <v>1052478</v>
       </c>
       <c r="D647">
-        <v>11559.24</v>
+        <v>189446.04</v>
       </c>
       <c r="E647">
-        <v>75777</v>
+        <v>1241924</v>
       </c>
       <c r="F647">
-        <v>9.73</v>
+        <v>167.06</v>
       </c>
       <c r="G647">
-        <v>6600</v>
+        <v>6300</v>
       </c>
       <c r="H647">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I647" t="inlineStr">
         <is>
@@ -24955,37 +24955,37 @@
         </is>
       </c>
       <c r="J647" s="2">
-        <v>45047</v>
+        <v>45078</v>
       </c>
     </row>
     <row r="648">
       <c r="A648" t="inlineStr">
         <is>
-          <t>Rama Hi Power Tech</t>
+          <t>Adishakti Smelters Private Limited</t>
         </is>
       </c>
       <c r="B648" t="inlineStr">
         <is>
-          <t>Nali Top</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C648">
-        <v>15640</v>
+        <v>591710</v>
       </c>
       <c r="D648">
-        <v>13815</v>
+        <v>106507.86</v>
       </c>
       <c r="E648">
-        <v>18455.2</v>
+        <v>698219</v>
       </c>
       <c r="F648">
-        <v>4.6</v>
+        <v>149.8</v>
       </c>
       <c r="G648">
-        <v>3400</v>
+        <v>3950</v>
       </c>
       <c r="H648">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I648" t="inlineStr">
         <is>
@@ -24993,75 +24993,75 @@
         </is>
       </c>
       <c r="J648" s="2">
-        <v>45047</v>
+        <v>45078</v>
       </c>
     </row>
     <row r="649">
       <c r="A649" t="inlineStr">
         <is>
-          <t>SHRADDHA ISPAT-MELTING DIVISION</t>
+          <t>Tulsyan NEC Limited</t>
         </is>
       </c>
       <c r="B649" t="inlineStr">
         <is>
-          <t>Nali Top</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C649">
-        <v>6800</v>
+        <v>1076554.5</v>
       </c>
       <c r="D649">
-        <v>6800</v>
+        <v>193779.81</v>
       </c>
       <c r="E649">
-        <v>7140</v>
+        <v>1270335</v>
       </c>
       <c r="F649">
-        <v>2</v>
+        <v>142.59</v>
       </c>
       <c r="G649">
-        <v>3400</v>
+        <v>7550</v>
       </c>
       <c r="H649">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I649" t="inlineStr">
         <is>
-          <t>Sunil Rathi</t>
+          <t>Abhijit Maloo</t>
         </is>
       </c>
       <c r="J649" s="2">
-        <v>45047</v>
+        <v>45078</v>
       </c>
     </row>
     <row r="650">
       <c r="A650" t="inlineStr">
         <is>
-          <t>SAMKRG PISTONS AND RINGS LIMITED</t>
+          <t>A One Ispat Private Ltd</t>
         </is>
       </c>
       <c r="B650" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C650">
-        <v>9920</v>
+        <v>1116586</v>
       </c>
       <c r="D650">
-        <v>1785.6</v>
+        <v>200985.48</v>
       </c>
       <c r="E650">
-        <v>11706</v>
+        <v>1317571</v>
       </c>
       <c r="F650">
-        <v>1.24</v>
+        <v>141.34</v>
       </c>
       <c r="G650">
-        <v>8000</v>
+        <v>7900</v>
       </c>
       <c r="H650">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I650" t="inlineStr">
         <is>
@@ -25069,13 +25069,13 @@
         </is>
       </c>
       <c r="J650" s="2">
-        <v>45047</v>
+        <v>45078</v>
       </c>
     </row>
     <row r="651">
       <c r="A651" t="inlineStr">
         <is>
-          <t>BMM ISPAT LIMITED</t>
+          <t>Mahrishi Alloys Pvt. Ltd.</t>
         </is>
       </c>
       <c r="B651" t="inlineStr">
@@ -25084,22 +25084,22 @@
         </is>
       </c>
       <c r="C651">
-        <v>1835137</v>
+        <v>309010</v>
       </c>
       <c r="D651">
-        <v>330324.66</v>
+        <v>55621.8</v>
       </c>
       <c r="E651">
-        <v>2165462</v>
+        <v>364632</v>
       </c>
       <c r="F651">
-        <v>258.47</v>
+        <v>95.08</v>
       </c>
       <c r="G651">
-        <v>7100.000000000001</v>
+        <v>3250</v>
       </c>
       <c r="H651">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I651" t="inlineStr">
         <is>
@@ -25113,35 +25113,35 @@
     <row r="652">
       <c r="A652" t="inlineStr">
         <is>
-          <t>Minera Steel &amp; Power Pvt Ltd</t>
+          <t>Mahalakshmi Profiles Pvt Ltd</t>
         </is>
       </c>
       <c r="B652" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C652">
-        <v>2154348</v>
+        <v>672987</v>
       </c>
       <c r="D652">
-        <v>387782.64</v>
+        <v>121137.66</v>
       </c>
       <c r="E652">
-        <v>2542130</v>
+        <v>794125</v>
       </c>
       <c r="F652">
-        <v>256.47</v>
+        <v>92.19</v>
       </c>
       <c r="G652">
-        <v>8400</v>
+        <v>7300</v>
       </c>
       <c r="H652">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I652" t="inlineStr">
         <is>
-          <t>Vishnu Kankani</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J652" s="2">
@@ -25151,7 +25151,7 @@
     <row r="653">
       <c r="A653" t="inlineStr">
         <is>
-          <t>Pushpit Steels Private Limited</t>
+          <t>Pulkit Metals Pvt Ltd</t>
         </is>
       </c>
       <c r="B653" t="inlineStr">
@@ -25160,22 +25160,22 @@
         </is>
       </c>
       <c r="C653">
-        <v>1058402</v>
+        <v>456900</v>
       </c>
       <c r="D653">
-        <v>190512.36</v>
+        <v>82242</v>
       </c>
       <c r="E653">
-        <v>1248913</v>
+        <v>539142</v>
       </c>
       <c r="F653">
-        <v>170.71</v>
+        <v>76.15000000000001</v>
       </c>
       <c r="G653">
-        <v>6200</v>
+        <v>6000</v>
       </c>
       <c r="H653">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I653" t="inlineStr">
         <is>
@@ -25189,31 +25189,31 @@
     <row r="654">
       <c r="A654" t="inlineStr">
         <is>
-          <t>Suryadev Alloys &amp; Power Pvt Ltd Quartztech</t>
+          <t>A One Steels And Alloys Pvt Ltd</t>
         </is>
       </c>
       <c r="B654" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C654">
-        <v>1052478</v>
+        <v>627456</v>
       </c>
       <c r="D654">
-        <v>189446.04</v>
+        <v>112942.08</v>
       </c>
       <c r="E654">
-        <v>1241924</v>
+        <v>740398</v>
       </c>
       <c r="F654">
-        <v>167.06</v>
+        <v>72.96000000000001</v>
       </c>
       <c r="G654">
-        <v>6300</v>
+        <v>8599.999999999998</v>
       </c>
       <c r="H654">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I654" t="inlineStr">
         <is>
@@ -25227,35 +25227,35 @@
     <row r="655">
       <c r="A655" t="inlineStr">
         <is>
-          <t>Tulsyan NEC Limited</t>
+          <t>Shri Tirupati Steel Cast Ltd</t>
         </is>
       </c>
       <c r="B655" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C655">
-        <v>1076554.5</v>
+        <v>227904</v>
       </c>
       <c r="D655">
-        <v>193779.81</v>
+        <v>41022.72</v>
       </c>
       <c r="E655">
-        <v>1270335</v>
+        <v>268928</v>
       </c>
       <c r="F655">
-        <v>142.59</v>
+        <v>71.22</v>
       </c>
       <c r="G655">
-        <v>7550</v>
+        <v>3200</v>
       </c>
       <c r="H655">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I655" t="inlineStr">
         <is>
-          <t>Abhijit Maloo</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J655" s="2">
@@ -25265,7 +25265,7 @@
     <row r="656">
       <c r="A656" t="inlineStr">
         <is>
-          <t>A One Ispat Private Ltd</t>
+          <t>Meenakshi Udyog India Pvt Ltd.</t>
         </is>
       </c>
       <c r="B656" t="inlineStr">
@@ -25274,26 +25274,26 @@
         </is>
       </c>
       <c r="C656">
-        <v>1116586</v>
+        <v>540072</v>
       </c>
       <c r="D656">
-        <v>200985.48</v>
+        <v>97212.96000000001</v>
       </c>
       <c r="E656">
-        <v>1317571</v>
+        <v>637284</v>
       </c>
       <c r="F656">
-        <v>141.34</v>
+        <v>69.24000000000001</v>
       </c>
       <c r="G656">
-        <v>7900</v>
+        <v>7799.999999999999</v>
       </c>
       <c r="H656">
         <v>4</v>
       </c>
       <c r="I656" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Abhijit Maloo</t>
         </is>
       </c>
       <c r="J656" s="2">
@@ -25303,35 +25303,35 @@
     <row r="657">
       <c r="A657" t="inlineStr">
         <is>
-          <t>Suryadev Alloys &amp; Power Pvt Ltd</t>
+          <t>JEPPIAAR FURNACE AND STEELS PVT.LTD</t>
         </is>
       </c>
       <c r="B657" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C657">
-        <v>928950</v>
+        <v>611616</v>
       </c>
       <c r="D657">
-        <v>167211</v>
+        <v>110090.88</v>
       </c>
       <c r="E657">
-        <v>1096162</v>
+        <v>721707</v>
       </c>
       <c r="F657">
-        <v>123.86</v>
+        <v>66.48</v>
       </c>
       <c r="G657">
-        <v>7500</v>
+        <v>9200</v>
       </c>
       <c r="H657">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I657" t="inlineStr">
         <is>
-          <t>Abhijit Maloo</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J657" s="2">
@@ -25341,7 +25341,7 @@
     <row r="658">
       <c r="A658" t="inlineStr">
         <is>
-          <t>Adishakti Smelters Private Limited</t>
+          <t>A One Steels And Alloys Pvt Ltd(A One Bellary)</t>
         </is>
       </c>
       <c r="B658" t="inlineStr">
@@ -25350,22 +25350,22 @@
         </is>
       </c>
       <c r="C658">
-        <v>444414.5</v>
+        <v>562096</v>
       </c>
       <c r="D658">
-        <v>79994.66</v>
+        <v>101177.28</v>
       </c>
       <c r="E658">
-        <v>524410</v>
+        <v>663273</v>
       </c>
       <c r="F658">
-        <v>112.51</v>
+        <v>65.36</v>
       </c>
       <c r="G658">
-        <v>3950</v>
+        <v>8600</v>
       </c>
       <c r="H658">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I658" t="inlineStr">
         <is>
@@ -25379,7 +25379,7 @@
     <row r="659">
       <c r="A659" t="inlineStr">
         <is>
-          <t>Mahrishi Alloys Pvt. Ltd.</t>
+          <t>GOVAAN STEELS PRIVATE LIMITED Quartztech</t>
         </is>
       </c>
       <c r="B659" t="inlineStr">
@@ -25388,22 +25388,22 @@
         </is>
       </c>
       <c r="C659">
-        <v>309010</v>
+        <v>390033</v>
       </c>
       <c r="D659">
-        <v>55621.8</v>
+        <v>70205.94</v>
       </c>
       <c r="E659">
-        <v>364632</v>
+        <v>460239</v>
       </c>
       <c r="F659">
-        <v>95.08</v>
+        <v>61.91</v>
       </c>
       <c r="G659">
-        <v>3250</v>
+        <v>6300</v>
       </c>
       <c r="H659">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I659" t="inlineStr">
         <is>
@@ -25417,7 +25417,7 @@
     <row r="660">
       <c r="A660" t="inlineStr">
         <is>
-          <t>Mahalakshmi Profiles Pvt Ltd</t>
+          <t>Shivam Ispat (P) Ltd</t>
         </is>
       </c>
       <c r="B660" t="inlineStr">
@@ -25426,26 +25426,26 @@
         </is>
       </c>
       <c r="C660">
-        <v>672987</v>
+        <v>365199</v>
       </c>
       <c r="D660">
-        <v>121137.66</v>
+        <v>65735.82000000001</v>
       </c>
       <c r="E660">
-        <v>794125</v>
+        <v>430935</v>
       </c>
       <c r="F660">
-        <v>92.19</v>
+        <v>56.62</v>
       </c>
       <c r="G660">
-        <v>7300</v>
+        <v>6449.999999999999</v>
       </c>
       <c r="H660">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I660" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Sunil Rathi</t>
         </is>
       </c>
       <c r="J660" s="2">
@@ -25455,35 +25455,35 @@
     <row r="661">
       <c r="A661" t="inlineStr">
         <is>
-          <t>A One Steels And Alloys Pvt Ltd</t>
+          <t>ILC IRON &amp; STEEL PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="B661" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C661">
-        <v>627456</v>
+        <v>335012</v>
       </c>
       <c r="D661">
-        <v>112942.08</v>
+        <v>38166.48</v>
       </c>
       <c r="E661">
-        <v>740398</v>
+        <v>395313.68</v>
       </c>
       <c r="F661">
-        <v>72.96000000000001</v>
+        <v>54.92</v>
       </c>
       <c r="G661">
-        <v>8599.999999999998</v>
+        <v>6100</v>
       </c>
       <c r="H661">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I661" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Shresth Maheshwari</t>
         </is>
       </c>
       <c r="J661" s="2">
@@ -25493,31 +25493,31 @@
     <row r="662">
       <c r="A662" t="inlineStr">
         <is>
-          <t>Shri Tirupati Steel Cast Ltd</t>
+          <t>Bharat Heavy Electricals Limited</t>
         </is>
       </c>
       <c r="B662" t="inlineStr">
         <is>
-          <t>Nali Top</t>
+          <t>Quartz Powder</t>
         </is>
       </c>
       <c r="C662">
-        <v>227904</v>
+        <v>238896.45</v>
       </c>
       <c r="D662">
-        <v>41022.72</v>
+        <v>11944.82</v>
       </c>
       <c r="E662">
-        <v>268928</v>
+        <v>250841</v>
       </c>
       <c r="F662">
-        <v>71.22</v>
+        <v>54.73</v>
       </c>
       <c r="G662">
-        <v>3200</v>
+        <v>4365</v>
       </c>
       <c r="H662">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I662" t="inlineStr">
         <is>
@@ -25531,35 +25531,35 @@
     <row r="663">
       <c r="A663" t="inlineStr">
         <is>
-          <t>Meenakshi Udyog India Pvt Ltd.</t>
+          <t>PURVA STEEL PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="B663" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C663">
-        <v>540072</v>
+        <v>292096</v>
       </c>
       <c r="D663">
-        <v>97212.96000000001</v>
+        <v>52577.28</v>
       </c>
       <c r="E663">
-        <v>637284</v>
+        <v>344673</v>
       </c>
       <c r="F663">
-        <v>69.24000000000001</v>
+        <v>45.64</v>
       </c>
       <c r="G663">
-        <v>7799.999999999999</v>
+        <v>6400</v>
       </c>
       <c r="H663">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I663" t="inlineStr">
         <is>
-          <t>Abhijit Maloo</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J663" s="2">
@@ -25569,35 +25569,35 @@
     <row r="664">
       <c r="A664" t="inlineStr">
         <is>
-          <t>JEPPIAAR FURNACE AND STEELS PVT.LTD</t>
+          <t>SHRADDHA ISPAT-MELTING DIVISION</t>
         </is>
       </c>
       <c r="B664" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C664">
-        <v>611616</v>
+        <v>257920</v>
       </c>
       <c r="D664">
-        <v>110090.88</v>
+        <v>46425.6</v>
       </c>
       <c r="E664">
-        <v>721707</v>
+        <v>304345.24</v>
       </c>
       <c r="F664">
-        <v>66.48</v>
+        <v>40.3</v>
       </c>
       <c r="G664">
-        <v>9200</v>
+        <v>6400</v>
       </c>
       <c r="H664">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I664" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Sunil Rathi</t>
         </is>
       </c>
       <c r="J664" s="2">
@@ -25607,35 +25607,35 @@
     <row r="665">
       <c r="A665" t="inlineStr">
         <is>
-          <t>A One Steels And Alloys Pvt Ltd(A One Bellary)</t>
+          <t>Orange Fox Steel Pvt Ltd(Cuncolim)</t>
         </is>
       </c>
       <c r="B665" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C665">
-        <v>562096</v>
+        <v>250518</v>
       </c>
       <c r="D665">
-        <v>101177.28</v>
+        <v>45093.24</v>
       </c>
       <c r="E665">
-        <v>663273</v>
+        <v>295611.74</v>
       </c>
       <c r="F665">
-        <v>65.36</v>
+        <v>38.84</v>
       </c>
       <c r="G665">
-        <v>8600</v>
+        <v>6449.999999999999</v>
       </c>
       <c r="H665">
         <v>2</v>
       </c>
       <c r="I665" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Sunil Rathi</t>
         </is>
       </c>
       <c r="J665" s="2">
@@ -25645,35 +25645,35 @@
     <row r="666">
       <c r="A666" t="inlineStr">
         <is>
-          <t>Shivam Ispat (P) Ltd</t>
+          <t>M S METALS AND STEELS PVT LTD (ANCHEPALYA)(M S METALS AND STEELS PVT LTD (Kunigal))</t>
         </is>
       </c>
       <c r="B666" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C666">
-        <v>365199</v>
+        <v>288240</v>
       </c>
       <c r="D666">
-        <v>65735.82000000001</v>
+        <v>51883.2</v>
       </c>
       <c r="E666">
-        <v>430935</v>
+        <v>340123</v>
       </c>
       <c r="F666">
-        <v>56.62</v>
+        <v>36.03</v>
       </c>
       <c r="G666">
-        <v>6449.999999999999</v>
+        <v>8000</v>
       </c>
       <c r="H666">
         <v>2</v>
       </c>
       <c r="I666" t="inlineStr">
         <is>
-          <t>Sunil Rathi</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J666" s="2">
@@ -25683,35 +25683,35 @@
     <row r="667">
       <c r="A667" t="inlineStr">
         <is>
-          <t>ILC IRON &amp; STEEL PRIVATE LIMITED</t>
+          <t>SHRADDHA ISPAT-MELTING DIVISION(SHRADDHA ISPAT PVT. LTD.)</t>
         </is>
       </c>
       <c r="B667" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C667">
-        <v>335012</v>
+        <v>121142</v>
       </c>
       <c r="D667">
-        <v>38166.48</v>
+        <v>21805.56</v>
       </c>
       <c r="E667">
-        <v>395313.68</v>
+        <v>142948</v>
       </c>
       <c r="F667">
-        <v>54.92</v>
+        <v>35.63</v>
       </c>
       <c r="G667">
-        <v>6100</v>
+        <v>3400</v>
       </c>
       <c r="H667">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I667" t="inlineStr">
         <is>
-          <t>Shresth Maheshwari</t>
+          <t>Sunil Rathi</t>
         </is>
       </c>
       <c r="J667" s="2">
@@ -25721,28 +25721,28 @@
     <row r="668">
       <c r="A668" t="inlineStr">
         <is>
-          <t>Bharat Heavy Electricals Limited</t>
+          <t>A One Steels And Alloys Pvt Ltd(A One Bellary)</t>
         </is>
       </c>
       <c r="B668" t="inlineStr">
         <is>
-          <t>Quartz Powder</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C668">
-        <v>238896.45</v>
+        <v>244918</v>
       </c>
       <c r="D668">
-        <v>11944.82</v>
+        <v>44085.24</v>
       </c>
       <c r="E668">
-        <v>250841</v>
+        <v>289003</v>
       </c>
       <c r="F668">
-        <v>54.73</v>
+        <v>35.24</v>
       </c>
       <c r="G668">
-        <v>4365</v>
+        <v>6950</v>
       </c>
       <c r="H668">
         <v>2</v>
@@ -25759,35 +25759,35 @@
     <row r="669">
       <c r="A669" t="inlineStr">
         <is>
-          <t>SHRADDHA ISPAT-MELTING DIVISION</t>
+          <t>Prakash Sponge Iron &amp; Power Pvt Ltd</t>
         </is>
       </c>
       <c r="B669" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C669">
-        <v>257920</v>
+        <v>267368</v>
       </c>
       <c r="D669">
-        <v>46425.6</v>
+        <v>48126.24</v>
       </c>
       <c r="E669">
-        <v>304345.24</v>
+        <v>315494</v>
       </c>
       <c r="F669">
-        <v>40.3</v>
+        <v>35.18</v>
       </c>
       <c r="G669">
-        <v>6400</v>
+        <v>7600</v>
       </c>
       <c r="H669">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I669" t="inlineStr">
         <is>
-          <t>Sunil Rathi</t>
+          <t>Shresth Maheshwari</t>
         </is>
       </c>
       <c r="J669" s="2">
@@ -25797,35 +25797,35 @@
     <row r="670">
       <c r="A670" t="inlineStr">
         <is>
-          <t>Orange Fox Steel Pvt Ltd(Cuncolim)</t>
+          <t>M S METALS AND STEELS PVT LTD (ANCHEPALYA)</t>
         </is>
       </c>
       <c r="B670" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C670">
-        <v>250518</v>
+        <v>277920</v>
       </c>
       <c r="D670">
-        <v>45093.24</v>
+        <v>50025.6</v>
       </c>
       <c r="E670">
-        <v>295611.74</v>
+        <v>327946</v>
       </c>
       <c r="F670">
-        <v>38.84</v>
+        <v>34.73999999999999</v>
       </c>
       <c r="G670">
-        <v>6449.999999999999</v>
+        <v>8000.000000000001</v>
       </c>
       <c r="H670">
         <v>2</v>
       </c>
       <c r="I670" t="inlineStr">
         <is>
-          <t>Sunil Rathi</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J670" s="2">
@@ -25835,7 +25835,7 @@
     <row r="671">
       <c r="A671" t="inlineStr">
         <is>
-          <t>M S METALS AND STEELS PVT LTD (ANCHEPALYA)(M S METALS AND STEELS PVT LTD (Kunigal))</t>
+          <t>Prime Gold International Limited</t>
         </is>
       </c>
       <c r="B671" t="inlineStr">
@@ -25844,26 +25844,26 @@
         </is>
       </c>
       <c r="C671">
-        <v>288240</v>
+        <v>276400</v>
       </c>
       <c r="D671">
-        <v>51883.2</v>
+        <v>49752</v>
       </c>
       <c r="E671">
-        <v>340123</v>
+        <v>326152</v>
       </c>
       <c r="F671">
-        <v>36.03</v>
+        <v>34.55</v>
       </c>
       <c r="G671">
-        <v>8000</v>
+        <v>8000.000000000001</v>
       </c>
       <c r="H671">
         <v>2</v>
       </c>
       <c r="I671" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Sharad Bhutra</t>
         </is>
       </c>
       <c r="J671" s="2">
@@ -25873,7 +25873,7 @@
     <row r="672">
       <c r="A672" t="inlineStr">
         <is>
-          <t>Pulkit Metals Pvt Ltd</t>
+          <t>Laxmi Rolling &amp; Strips Pvt Ltd</t>
         </is>
       </c>
       <c r="B672" t="inlineStr">
@@ -25882,26 +25882,26 @@
         </is>
       </c>
       <c r="C672">
-        <v>213840</v>
+        <v>217350</v>
       </c>
       <c r="D672">
-        <v>38491.2</v>
+        <v>39123</v>
       </c>
       <c r="E672">
-        <v>252331</v>
+        <v>256473</v>
       </c>
       <c r="F672">
-        <v>35.64</v>
+        <v>34.5</v>
       </c>
       <c r="G672">
-        <v>6000</v>
+        <v>6300</v>
       </c>
       <c r="H672">
         <v>2</v>
       </c>
       <c r="I672" t="inlineStr">
         <is>
-          <t>Abhijit Maloo</t>
+          <t>Shresth Maheshwari</t>
         </is>
       </c>
       <c r="J672" s="2">
@@ -25911,7 +25911,7 @@
     <row r="673">
       <c r="A673" t="inlineStr">
         <is>
-          <t>SHRADDHA ISPAT-MELTING DIVISION(SHRADDHA ISPAT PVT. LTD.)</t>
+          <t>Mahrishi Alloys Pvt. Ltd.</t>
         </is>
       </c>
       <c r="B673" t="inlineStr">
@@ -25920,26 +25920,26 @@
         </is>
       </c>
       <c r="C673">
-        <v>121142</v>
+        <v>52142</v>
       </c>
       <c r="D673">
-        <v>21805.56</v>
+        <v>9385.58</v>
       </c>
       <c r="E673">
-        <v>142948</v>
+        <v>61528</v>
       </c>
       <c r="F673">
-        <v>35.63</v>
+        <v>33.64</v>
       </c>
       <c r="G673">
-        <v>3400</v>
+        <v>1550</v>
       </c>
       <c r="H673">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I673" t="inlineStr">
         <is>
-          <t>Sunil Rathi</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J673" s="2">
@@ -25949,31 +25949,31 @@
     <row r="674">
       <c r="A674" t="inlineStr">
         <is>
-          <t>A One Steels And Alloys Pvt Ltd(A One Bellary)</t>
+          <t>A One Steel &amp; Alloys Pvt Ltd.(A One Steel (GBD))</t>
         </is>
       </c>
       <c r="B674" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C674">
-        <v>244918</v>
+        <v>256387.5</v>
       </c>
       <c r="D674">
-        <v>44085.24</v>
+        <v>46149.75</v>
       </c>
       <c r="E674">
-        <v>289003</v>
+        <v>302537</v>
       </c>
       <c r="F674">
-        <v>35.24</v>
+        <v>32.25</v>
       </c>
       <c r="G674">
-        <v>6950</v>
+        <v>7950</v>
       </c>
       <c r="H674">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I674" t="inlineStr">
         <is>
@@ -25987,35 +25987,35 @@
     <row r="675">
       <c r="A675" t="inlineStr">
         <is>
-          <t>Prakash Sponge Iron &amp; Power Pvt Ltd</t>
+          <t>Sugna Sponge &amp; Power Pvt Ltd</t>
         </is>
       </c>
       <c r="B675" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C675">
-        <v>267368</v>
+        <v>102688</v>
       </c>
       <c r="D675">
-        <v>48126.24</v>
+        <v>18483.84</v>
       </c>
       <c r="E675">
-        <v>315494</v>
+        <v>121172</v>
       </c>
       <c r="F675">
-        <v>35.18</v>
+        <v>32.09</v>
       </c>
       <c r="G675">
-        <v>7600</v>
+        <v>3200</v>
       </c>
       <c r="H675">
         <v>1</v>
       </c>
       <c r="I675" t="inlineStr">
         <is>
-          <t>Shresth Maheshwari</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J675" s="2">
@@ -26025,35 +26025,35 @@
     <row r="676">
       <c r="A676" t="inlineStr">
         <is>
-          <t>M S METALS AND STEELS PVT LTD (ANCHEPALYA)</t>
+          <t>Sri Vinayaga Alloys (P) Ltd</t>
         </is>
       </c>
       <c r="B676" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C676">
-        <v>277920</v>
+        <v>195741</v>
       </c>
       <c r="D676">
-        <v>50025.6</v>
+        <v>35233.38</v>
       </c>
       <c r="E676">
-        <v>327946</v>
+        <v>230974</v>
       </c>
       <c r="F676">
-        <v>34.73999999999999</v>
+        <v>31.07</v>
       </c>
       <c r="G676">
-        <v>8000.000000000001</v>
+        <v>6300</v>
       </c>
       <c r="H676">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I676" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Vishnu Kankani</t>
         </is>
       </c>
       <c r="J676" s="2">
@@ -26063,35 +26063,35 @@
     <row r="677">
       <c r="A677" t="inlineStr">
         <is>
-          <t>Prime Gold International Limited</t>
+          <t>M.A.STEELS (P) LTD</t>
         </is>
       </c>
       <c r="B677" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C677">
-        <v>276400</v>
+        <v>194985</v>
       </c>
       <c r="D677">
-        <v>49752</v>
+        <v>35097.3</v>
       </c>
       <c r="E677">
-        <v>326152</v>
+        <v>230082</v>
       </c>
       <c r="F677">
-        <v>34.55</v>
+        <v>30.95</v>
       </c>
       <c r="G677">
-        <v>8000.000000000001</v>
+        <v>6300</v>
       </c>
       <c r="H677">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I677" t="inlineStr">
         <is>
-          <t>Sharad Bhutra</t>
+          <t>Vishnu Kankani</t>
         </is>
       </c>
       <c r="J677" s="2">
@@ -26101,7 +26101,7 @@
     <row r="678">
       <c r="A678" t="inlineStr">
         <is>
-          <t>Laxmi Rolling &amp; Strips Pvt Ltd</t>
+          <t>PREMIUM FERRO ALLOYS LIMITED</t>
         </is>
       </c>
       <c r="B678" t="inlineStr">
@@ -26110,26 +26110,26 @@
         </is>
       </c>
       <c r="C678">
-        <v>217350</v>
+        <v>194733</v>
       </c>
       <c r="D678">
-        <v>39123</v>
+        <v>35051.94</v>
       </c>
       <c r="E678">
-        <v>256473</v>
+        <v>229785</v>
       </c>
       <c r="F678">
-        <v>34.5</v>
+        <v>30.91</v>
       </c>
       <c r="G678">
         <v>6300</v>
       </c>
       <c r="H678">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I678" t="inlineStr">
         <is>
-          <t>Shresth Maheshwari</t>
+          <t>Vishnu Kankani</t>
         </is>
       </c>
       <c r="J678" s="2">
@@ -26139,35 +26139,35 @@
     <row r="679">
       <c r="A679" t="inlineStr">
         <is>
-          <t>Mahrishi Alloys Pvt. Ltd.</t>
+          <t>GOVAAN STEELS PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="B679" t="inlineStr">
         <is>
-          <t>Nali Top</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C679">
-        <v>52142</v>
+        <v>197376</v>
       </c>
       <c r="D679">
-        <v>9385.58</v>
+        <v>35527.68</v>
       </c>
       <c r="E679">
-        <v>61528</v>
+        <v>232904</v>
       </c>
       <c r="F679">
-        <v>33.64</v>
+        <v>30.84</v>
       </c>
       <c r="G679">
-        <v>1550</v>
+        <v>6400</v>
       </c>
       <c r="H679">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I679" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Vishnu Kankani</t>
         </is>
       </c>
       <c r="J679" s="2">
@@ -26177,35 +26177,35 @@
     <row r="680">
       <c r="A680" t="inlineStr">
         <is>
-          <t>A One Steel &amp; Alloys Pvt Ltd.(A One Steel (GBD))</t>
+          <t>Sri Vigneshwara Steels (p) Ltd</t>
         </is>
       </c>
       <c r="B680" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C680">
-        <v>256387.5</v>
+        <v>190827</v>
       </c>
       <c r="D680">
-        <v>46149.75</v>
+        <v>34348.86</v>
       </c>
       <c r="E680">
-        <v>302537</v>
+        <v>225176</v>
       </c>
       <c r="F680">
-        <v>32.25</v>
+        <v>30.29</v>
       </c>
       <c r="G680">
-        <v>7950</v>
+        <v>6300</v>
       </c>
       <c r="H680">
         <v>1</v>
       </c>
       <c r="I680" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Vishnu Kankani</t>
         </is>
       </c>
       <c r="J680" s="2">
@@ -26215,28 +26215,28 @@
     <row r="681">
       <c r="A681" t="inlineStr">
         <is>
-          <t>Sugna Sponge &amp; Power Pvt Ltd</t>
+          <t>Oswal Smelters Pvt Ltd</t>
         </is>
       </c>
       <c r="B681" t="inlineStr">
         <is>
-          <t>Nali Top</t>
+          <t>Quartz Grain</t>
         </is>
       </c>
       <c r="C681">
-        <v>102688</v>
+        <v>147000</v>
       </c>
       <c r="D681">
-        <v>18483.84</v>
+        <v>7350</v>
       </c>
       <c r="E681">
-        <v>121172</v>
+        <v>154350</v>
       </c>
       <c r="F681">
-        <v>32.09</v>
+        <v>30</v>
       </c>
       <c r="G681">
-        <v>3200</v>
+        <v>4900</v>
       </c>
       <c r="H681">
         <v>1</v>
@@ -26253,7 +26253,7 @@
     <row r="682">
       <c r="A682" t="inlineStr">
         <is>
-          <t>Quartztech Minerals Pvt Ltd</t>
+          <t>ILC IRON &amp; STEEL PRIVATE LIMITED(ILC IRON &amp; STEEL PRIVATE LIMITED (Hospet))</t>
         </is>
       </c>
       <c r="B682" t="inlineStr">
@@ -26262,26 +26262,26 @@
         </is>
       </c>
       <c r="C682">
-        <v>198765</v>
+        <v>181109</v>
       </c>
       <c r="D682">
-        <v>35777.7</v>
+        <v>32599.62</v>
       </c>
       <c r="E682">
-        <v>234543</v>
+        <v>213709</v>
       </c>
       <c r="F682">
-        <v>31.55</v>
+        <v>29.69</v>
       </c>
       <c r="G682">
-        <v>6300</v>
+        <v>6100</v>
       </c>
       <c r="H682">
         <v>1</v>
       </c>
       <c r="I682" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Shresth Maheshwari</t>
         </is>
       </c>
       <c r="J682" s="2">
@@ -26291,35 +26291,35 @@
     <row r="683">
       <c r="A683" t="inlineStr">
         <is>
-          <t>Sri Vinayaga Alloys (P) Ltd</t>
+          <t>Mahrishi Alloys Pvt. Ltd.</t>
         </is>
       </c>
       <c r="B683" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Quartz Powder</t>
         </is>
       </c>
       <c r="C683">
-        <v>195741</v>
+        <v>15581.5</v>
       </c>
       <c r="D683">
-        <v>35233.38</v>
+        <v>779.08</v>
       </c>
       <c r="E683">
-        <v>230974</v>
+        <v>16361</v>
       </c>
       <c r="F683">
-        <v>31.07</v>
+        <v>28.33</v>
       </c>
       <c r="G683">
-        <v>6300</v>
+        <v>550</v>
       </c>
       <c r="H683">
         <v>1</v>
       </c>
       <c r="I683" t="inlineStr">
         <is>
-          <t>Vishnu Kankani</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J683" s="2">
@@ -26329,7 +26329,7 @@
     <row r="684">
       <c r="A684" t="inlineStr">
         <is>
-          <t>M.A.STEELS (P) LTD</t>
+          <t>MINAR ISPAT PVT. LTD</t>
         </is>
       </c>
       <c r="B684" t="inlineStr">
@@ -26338,26 +26338,26 @@
         </is>
       </c>
       <c r="C684">
-        <v>194985</v>
+        <v>157377.5</v>
       </c>
       <c r="D684">
-        <v>35097.3</v>
+        <v>28327.95</v>
       </c>
       <c r="E684">
-        <v>230082</v>
+        <v>185705</v>
       </c>
       <c r="F684">
-        <v>30.95</v>
+        <v>26.45</v>
       </c>
       <c r="G684">
-        <v>6300</v>
+        <v>5950</v>
       </c>
       <c r="H684">
         <v>1</v>
       </c>
       <c r="I684" t="inlineStr">
         <is>
-          <t>Vishnu Kankani</t>
+          <t>Abhijit Maloo</t>
         </is>
       </c>
       <c r="J684" s="2">
@@ -26367,35 +26367,35 @@
     <row r="685">
       <c r="A685" t="inlineStr">
         <is>
-          <t>PREMIUM FERRO ALLOYS LIMITED</t>
+          <t>Ardex Endura (India) Private Ltd Quartztech</t>
         </is>
       </c>
       <c r="B685" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Quartz Powder</t>
         </is>
       </c>
       <c r="C685">
-        <v>194733</v>
+        <v>68000</v>
       </c>
       <c r="D685">
-        <v>35051.94</v>
+        <v>0</v>
       </c>
       <c r="E685">
-        <v>229785</v>
+        <v>71400</v>
       </c>
       <c r="F685">
-        <v>30.91</v>
+        <v>25</v>
       </c>
       <c r="G685">
-        <v>6300</v>
+        <v>2720</v>
       </c>
       <c r="H685">
         <v>1</v>
       </c>
       <c r="I685" t="inlineStr">
         <is>
-          <t>Vishnu Kankani</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J685" s="2">
@@ -26405,35 +26405,35 @@
     <row r="686">
       <c r="A686" t="inlineStr">
         <is>
-          <t>GOVAAN STEELS PRIVATE LIMITED</t>
+          <t>A One Steel &amp; Alloys Pvt Ltd.</t>
         </is>
       </c>
       <c r="B686" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C686">
-        <v>197376</v>
+        <v>158920.5</v>
       </c>
       <c r="D686">
-        <v>35527.68</v>
+        <v>28605.69</v>
       </c>
       <c r="E686">
-        <v>232904</v>
+        <v>187526</v>
       </c>
       <c r="F686">
-        <v>30.84</v>
+        <v>19.99</v>
       </c>
       <c r="G686">
-        <v>6400</v>
+        <v>7950.000000000001</v>
       </c>
       <c r="H686">
         <v>1</v>
       </c>
       <c r="I686" t="inlineStr">
         <is>
-          <t>Vishnu Kankani</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J686" s="2">
@@ -26443,28 +26443,28 @@
     <row r="687">
       <c r="A687" t="inlineStr">
         <is>
-          <t>PURVA STEEL PRIVATE LIMITED</t>
+          <t>Ardex Endura (India) Private Ltd</t>
         </is>
       </c>
       <c r="B687" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Quartz Powder</t>
         </is>
       </c>
       <c r="C687">
-        <v>194368</v>
+        <v>74960</v>
       </c>
       <c r="D687">
-        <v>34986.24</v>
+        <v>3748</v>
       </c>
       <c r="E687">
-        <v>229354</v>
+        <v>78708</v>
       </c>
       <c r="F687">
-        <v>30.37</v>
+        <v>18.74</v>
       </c>
       <c r="G687">
-        <v>6400</v>
+        <v>4000</v>
       </c>
       <c r="H687">
         <v>1</v>
@@ -26481,28 +26481,28 @@
     <row r="688">
       <c r="A688" t="inlineStr">
         <is>
-          <t>GOVAAN STEELS PRIVATE LIMITED Quartztech</t>
+          <t>PURVA STEEL PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="B688" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C688">
-        <v>191268</v>
+        <v>53108</v>
       </c>
       <c r="D688">
-        <v>34428.24</v>
+        <v>9559.440000000001</v>
       </c>
       <c r="E688">
-        <v>225696</v>
+        <v>62667</v>
       </c>
       <c r="F688">
-        <v>30.36</v>
+        <v>15.62</v>
       </c>
       <c r="G688">
-        <v>6300</v>
+        <v>3400</v>
       </c>
       <c r="H688">
         <v>1</v>
@@ -26519,28 +26519,28 @@
     <row r="689">
       <c r="A689" t="inlineStr">
         <is>
-          <t>Oswal Smelters Pvt Ltd</t>
+          <t>Rama Hi Power Tech</t>
         </is>
       </c>
       <c r="B689" t="inlineStr">
         <is>
-          <t>Quartz Grain</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C689">
-        <v>147000</v>
+        <v>69720</v>
       </c>
       <c r="D689">
-        <v>7350</v>
+        <v>12549.6</v>
       </c>
       <c r="E689">
-        <v>154350</v>
+        <v>82270</v>
       </c>
       <c r="F689">
-        <v>30</v>
+        <v>9.960000000000001</v>
       </c>
       <c r="G689">
-        <v>4900</v>
+        <v>6999.999999999999</v>
       </c>
       <c r="H689">
         <v>1</v>
@@ -26557,28 +26557,28 @@
     <row r="690">
       <c r="A690" t="inlineStr">
         <is>
-          <t>ILC IRON &amp; STEEL PRIVATE LIMITED(ILC IRON &amp; STEEL PRIVATE LIMITED (Hospet))</t>
+          <t>ILC IRON &amp; STEEL PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="B690" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C690">
-        <v>181109</v>
+        <v>29460</v>
       </c>
       <c r="D690">
-        <v>32599.62</v>
+        <v>27438.48</v>
       </c>
       <c r="E690">
-        <v>213709</v>
+        <v>30933</v>
       </c>
       <c r="F690">
-        <v>29.69</v>
+        <v>9.82</v>
       </c>
       <c r="G690">
-        <v>6100</v>
+        <v>3000</v>
       </c>
       <c r="H690">
         <v>1</v>
@@ -26595,28 +26595,28 @@
     <row r="691">
       <c r="A691" t="inlineStr">
         <is>
-          <t>Mahrishi Alloys Pvt. Ltd.</t>
+          <t>Adishakti Smelters Private Limited</t>
         </is>
       </c>
       <c r="B691" t="inlineStr">
         <is>
-          <t>Quartz Powder</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C691">
-        <v>15581.5</v>
+        <v>7296</v>
       </c>
       <c r="D691">
-        <v>779.08</v>
+        <v>1313.28</v>
       </c>
       <c r="E691">
-        <v>16361</v>
+        <v>8609</v>
       </c>
       <c r="F691">
-        <v>28.33</v>
+        <v>4.56</v>
       </c>
       <c r="G691">
-        <v>550</v>
+        <v>1600</v>
       </c>
       <c r="H691">
         <v>1</v>
@@ -26633,7 +26633,7 @@
     <row r="692">
       <c r="A692" t="inlineStr">
         <is>
-          <t>MINAR ISPAT PVT. LTD</t>
+          <t>HINDUSTAN AERONAUTICS LTD</t>
         </is>
       </c>
       <c r="B692" t="inlineStr">
@@ -26642,333 +26642,29 @@
         </is>
       </c>
       <c r="C692">
-        <v>157377.5</v>
+        <v>17710</v>
       </c>
       <c r="D692">
-        <v>28327.95</v>
+        <v>885.5</v>
       </c>
       <c r="E692">
-        <v>185705</v>
+        <v>18596</v>
       </c>
       <c r="F692">
-        <v>26.45</v>
+        <v>2.53</v>
       </c>
       <c r="G692">
-        <v>5950</v>
+        <v>7000.000000000001</v>
       </c>
       <c r="H692">
         <v>1</v>
       </c>
       <c r="I692" t="inlineStr">
         <is>
-          <t>Abhijit Maloo</t>
+          <t>Shresth Maheshwari</t>
         </is>
       </c>
       <c r="J692" s="2">
-        <v>45078</v>
-      </c>
-    </row>
-    <row r="693">
-      <c r="A693" t="inlineStr">
-        <is>
-          <t>Ardex Endura (India) Private Ltd Quartztech</t>
-        </is>
-      </c>
-      <c r="B693" t="inlineStr">
-        <is>
-          <t>Quartz Powder</t>
-        </is>
-      </c>
-      <c r="C693">
-        <v>68000</v>
-      </c>
-      <c r="D693">
-        <v>0</v>
-      </c>
-      <c r="E693">
-        <v>71400</v>
-      </c>
-      <c r="F693">
-        <v>25</v>
-      </c>
-      <c r="G693">
-        <v>2720</v>
-      </c>
-      <c r="H693">
-        <v>1</v>
-      </c>
-      <c r="I693" t="inlineStr">
-        <is>
-          <t>Direct</t>
-        </is>
-      </c>
-      <c r="J693" s="2">
-        <v>45078</v>
-      </c>
-    </row>
-    <row r="694">
-      <c r="A694" t="inlineStr">
-        <is>
-          <t>A One Steel &amp; Alloys Pvt Ltd.</t>
-        </is>
-      </c>
-      <c r="B694" t="inlineStr">
-        <is>
-          <t>Boron Oxide Premix</t>
-        </is>
-      </c>
-      <c r="C694">
-        <v>158920.5</v>
-      </c>
-      <c r="D694">
-        <v>28605.69</v>
-      </c>
-      <c r="E694">
-        <v>187526</v>
-      </c>
-      <c r="F694">
-        <v>19.99</v>
-      </c>
-      <c r="G694">
-        <v>7950.000000000001</v>
-      </c>
-      <c r="H694">
-        <v>1</v>
-      </c>
-      <c r="I694" t="inlineStr">
-        <is>
-          <t>Direct</t>
-        </is>
-      </c>
-      <c r="J694" s="2">
-        <v>45078</v>
-      </c>
-    </row>
-    <row r="695">
-      <c r="A695" t="inlineStr">
-        <is>
-          <t>Ardex Endura (India) Private Ltd</t>
-        </is>
-      </c>
-      <c r="B695" t="inlineStr">
-        <is>
-          <t>Quartz Powder</t>
-        </is>
-      </c>
-      <c r="C695">
-        <v>74960</v>
-      </c>
-      <c r="D695">
-        <v>3748</v>
-      </c>
-      <c r="E695">
-        <v>78708</v>
-      </c>
-      <c r="F695">
-        <v>18.74</v>
-      </c>
-      <c r="G695">
-        <v>4000</v>
-      </c>
-      <c r="H695">
-        <v>1</v>
-      </c>
-      <c r="I695" t="inlineStr">
-        <is>
-          <t>Direct</t>
-        </is>
-      </c>
-      <c r="J695" s="2">
-        <v>45078</v>
-      </c>
-    </row>
-    <row r="696">
-      <c r="A696" t="inlineStr">
-        <is>
-          <t>PURVA STEEL PRIVATE LIMITED</t>
-        </is>
-      </c>
-      <c r="B696" t="inlineStr">
-        <is>
-          <t>Nali Top</t>
-        </is>
-      </c>
-      <c r="C696">
-        <v>53108</v>
-      </c>
-      <c r="D696">
-        <v>9559.440000000001</v>
-      </c>
-      <c r="E696">
-        <v>62667</v>
-      </c>
-      <c r="F696">
-        <v>15.62</v>
-      </c>
-      <c r="G696">
-        <v>3400</v>
-      </c>
-      <c r="H696">
-        <v>1</v>
-      </c>
-      <c r="I696" t="inlineStr">
-        <is>
-          <t>Direct</t>
-        </is>
-      </c>
-      <c r="J696" s="2">
-        <v>45078</v>
-      </c>
-    </row>
-    <row r="697">
-      <c r="A697" t="inlineStr">
-        <is>
-          <t>Rama Hi Power Tech</t>
-        </is>
-      </c>
-      <c r="B697" t="inlineStr">
-        <is>
-          <t>Boric Acid Premix</t>
-        </is>
-      </c>
-      <c r="C697">
-        <v>69720</v>
-      </c>
-      <c r="D697">
-        <v>12549.6</v>
-      </c>
-      <c r="E697">
-        <v>82270</v>
-      </c>
-      <c r="F697">
-        <v>9.960000000000001</v>
-      </c>
-      <c r="G697">
-        <v>6999.999999999999</v>
-      </c>
-      <c r="H697">
-        <v>1</v>
-      </c>
-      <c r="I697" t="inlineStr">
-        <is>
-          <t>Direct</t>
-        </is>
-      </c>
-      <c r="J697" s="2">
-        <v>45078</v>
-      </c>
-    </row>
-    <row r="698">
-      <c r="A698" t="inlineStr">
-        <is>
-          <t>ILC IRON &amp; STEEL PRIVATE LIMITED</t>
-        </is>
-      </c>
-      <c r="B698" t="inlineStr">
-        <is>
-          <t>Nali Top</t>
-        </is>
-      </c>
-      <c r="C698">
-        <v>29460</v>
-      </c>
-      <c r="D698">
-        <v>27438.48</v>
-      </c>
-      <c r="E698">
-        <v>30933</v>
-      </c>
-      <c r="F698">
-        <v>9.82</v>
-      </c>
-      <c r="G698">
-        <v>3000</v>
-      </c>
-      <c r="H698">
-        <v>1</v>
-      </c>
-      <c r="I698" t="inlineStr">
-        <is>
-          <t>Shresth Maheshwari</t>
-        </is>
-      </c>
-      <c r="J698" s="2">
-        <v>45078</v>
-      </c>
-    </row>
-    <row r="699">
-      <c r="A699" t="inlineStr">
-        <is>
-          <t>Adishakti Smelters Private Limited</t>
-        </is>
-      </c>
-      <c r="B699" t="inlineStr">
-        <is>
-          <t>Nali Top</t>
-        </is>
-      </c>
-      <c r="C699">
-        <v>7296</v>
-      </c>
-      <c r="D699">
-        <v>1313.28</v>
-      </c>
-      <c r="E699">
-        <v>8609</v>
-      </c>
-      <c r="F699">
-        <v>4.56</v>
-      </c>
-      <c r="G699">
-        <v>1600</v>
-      </c>
-      <c r="H699">
-        <v>1</v>
-      </c>
-      <c r="I699" t="inlineStr">
-        <is>
-          <t>Direct</t>
-        </is>
-      </c>
-      <c r="J699" s="2">
-        <v>45078</v>
-      </c>
-    </row>
-    <row r="700">
-      <c r="A700" t="inlineStr">
-        <is>
-          <t>HINDUSTAN AERONAUTICS LTD</t>
-        </is>
-      </c>
-      <c r="B700" t="inlineStr">
-        <is>
-          <t>Boric Acid Premix</t>
-        </is>
-      </c>
-      <c r="C700">
-        <v>17710</v>
-      </c>
-      <c r="D700">
-        <v>885.5</v>
-      </c>
-      <c r="E700">
-        <v>18596</v>
-      </c>
-      <c r="F700">
-        <v>2.53</v>
-      </c>
-      <c r="G700">
-        <v>7000.000000000001</v>
-      </c>
-      <c r="H700">
-        <v>1</v>
-      </c>
-      <c r="I700" t="inlineStr">
-        <is>
-          <t>Shresth Maheshwari</t>
-        </is>
-      </c>
-      <c r="J700" s="2">
         <v>45078</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update for july 23'
</commit_message>
<xml_diff>
--- a/src/customers.xlsx
+++ b/src/customers.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J734"/>
+  <dimension ref="A1:J740"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -26984,22 +26984,22 @@
         </is>
       </c>
       <c r="C701">
-        <v>1647697</v>
+        <v>1859277</v>
       </c>
       <c r="D701">
         <v>296585.46</v>
       </c>
       <c r="E701">
-        <v>1944282.56</v>
+        <v>2193946.96</v>
       </c>
       <c r="F701">
-        <v>232.07</v>
+        <v>261.87</v>
       </c>
       <c r="G701">
         <v>7100</v>
       </c>
       <c r="H701">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I701" t="inlineStr">
         <is>
@@ -27060,22 +27060,22 @@
         </is>
       </c>
       <c r="C703">
-        <v>1188264</v>
+        <v>1485624</v>
       </c>
       <c r="D703">
         <v>213887.52</v>
       </c>
       <c r="E703">
-        <v>1402151.6</v>
+        <v>1753036.4</v>
       </c>
       <c r="F703">
-        <v>141.46</v>
+        <v>176.86</v>
       </c>
       <c r="G703">
         <v>8400</v>
       </c>
       <c r="H703">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I703" t="inlineStr">
         <is>
@@ -27089,35 +27089,35 @@
     <row r="704">
       <c r="A704" t="inlineStr">
         <is>
-          <t>Suryadev Alloys &amp; Power Pvt Ltd</t>
+          <t>Adishakti Smelters Private Limited</t>
         </is>
       </c>
       <c r="B704" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C704">
-        <v>1016175</v>
+        <v>610630.5</v>
       </c>
       <c r="D704">
-        <v>182911.5</v>
+        <v>93623.08</v>
       </c>
       <c r="E704">
-        <v>1199087</v>
+        <v>720543.86</v>
       </c>
       <c r="F704">
-        <v>135.49</v>
+        <v>154.59</v>
       </c>
       <c r="G704">
-        <v>7499.999999999999</v>
+        <v>3950</v>
       </c>
       <c r="H704">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I704" t="inlineStr">
         <is>
-          <t>Abhijit Maloo</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J704" s="2">
@@ -27127,35 +27127,35 @@
     <row r="705">
       <c r="A705" t="inlineStr">
         <is>
-          <t>Adishakti Smelters Private Limited</t>
+          <t>Suryadev Alloys &amp; Power Pvt Ltd</t>
         </is>
       </c>
       <c r="B705" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C705">
-        <v>491696</v>
+        <v>1016175</v>
       </c>
       <c r="D705">
-        <v>93623.08</v>
+        <v>182911.5</v>
       </c>
       <c r="E705">
-        <v>580201.15</v>
+        <v>1199087</v>
       </c>
       <c r="F705">
-        <v>124.48</v>
+        <v>135.49</v>
       </c>
       <c r="G705">
-        <v>3950</v>
+        <v>7499.999999999999</v>
       </c>
       <c r="H705">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I705" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Abhijit Maloo</t>
         </is>
       </c>
       <c r="J705" s="2">
@@ -27203,28 +27203,28 @@
     <row r="707">
       <c r="A707" t="inlineStr">
         <is>
-          <t>A One Steel &amp; Alloys Pvt Ltd.</t>
+          <t>Suryadev Alloys &amp; Power Pvt Ltd Quartztech</t>
         </is>
       </c>
       <c r="B707" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C707">
-        <v>754614</v>
+        <v>629811</v>
       </c>
       <c r="D707">
-        <v>135830.52</v>
+        <v>77588.28</v>
       </c>
       <c r="E707">
-        <v>890445</v>
+        <v>743176.7</v>
       </c>
       <c r="F707">
-        <v>94.92</v>
+        <v>99.97</v>
       </c>
       <c r="G707">
-        <v>7950</v>
+        <v>6299.999999999999</v>
       </c>
       <c r="H707">
         <v>3</v>
@@ -27241,7 +27241,7 @@
     <row r="708">
       <c r="A708" t="inlineStr">
         <is>
-          <t>A One Steels And Alloys Pvt Ltd</t>
+          <t>A One Steel &amp; Alloys Pvt Ltd.</t>
         </is>
       </c>
       <c r="B708" t="inlineStr">
@@ -27250,22 +27250,22 @@
         </is>
       </c>
       <c r="C708">
-        <v>717842</v>
+        <v>754614</v>
       </c>
       <c r="D708">
-        <v>129211.56</v>
+        <v>135830.52</v>
       </c>
       <c r="E708">
-        <v>847053</v>
+        <v>890445</v>
       </c>
       <c r="F708">
-        <v>83.47</v>
+        <v>94.92</v>
       </c>
       <c r="G708">
-        <v>8600</v>
+        <v>7950</v>
       </c>
       <c r="H708">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I708" t="inlineStr">
         <is>
@@ -27279,31 +27279,31 @@
     <row r="709">
       <c r="A709" t="inlineStr">
         <is>
-          <t>M S METALS AND STEELS PVT LTD (ANCHEPALYA)</t>
+          <t>Sri Navdurga Billets Pvt Ltd</t>
         </is>
       </c>
       <c r="B709" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C709">
-        <v>656480</v>
+        <v>612616</v>
       </c>
       <c r="D709">
-        <v>118166.4</v>
+        <v>46699.56</v>
       </c>
       <c r="E709">
-        <v>774646</v>
+        <v>722887.3200000001</v>
       </c>
       <c r="F709">
-        <v>82.06</v>
+        <v>83.92</v>
       </c>
       <c r="G709">
-        <v>8000</v>
+        <v>7300</v>
       </c>
       <c r="H709">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I709" t="inlineStr">
         <is>
@@ -27317,35 +27317,35 @@
     <row r="710">
       <c r="A710" t="inlineStr">
         <is>
-          <t>Shivam Ispat (P) Ltd</t>
+          <t>A One Steels And Alloys Pvt Ltd</t>
         </is>
       </c>
       <c r="B710" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C710">
-        <v>488329.5</v>
+        <v>717842</v>
       </c>
       <c r="D710">
-        <v>87899.31</v>
+        <v>129211.56</v>
       </c>
       <c r="E710">
-        <v>576228</v>
+        <v>847053</v>
       </c>
       <c r="F710">
-        <v>75.70999999999999</v>
+        <v>83.47</v>
       </c>
       <c r="G710">
-        <v>6450.000000000001</v>
+        <v>8600</v>
       </c>
       <c r="H710">
         <v>4</v>
       </c>
       <c r="I710" t="inlineStr">
         <is>
-          <t>Sunil Rathi</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J710" s="2">
@@ -27355,31 +27355,31 @@
     <row r="711">
       <c r="A711" t="inlineStr">
         <is>
-          <t>Suryadev Alloys &amp; Power Pvt Ltd Quartztech</t>
+          <t>M S METALS AND STEELS PVT LTD (ANCHEPALYA)</t>
         </is>
       </c>
       <c r="B711" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C711">
-        <v>431046</v>
+        <v>656480</v>
       </c>
       <c r="D711">
-        <v>77588.28</v>
+        <v>118166.4</v>
       </c>
       <c r="E711">
-        <v>508634</v>
+        <v>774646</v>
       </c>
       <c r="F711">
-        <v>68.42</v>
+        <v>82.06</v>
       </c>
       <c r="G711">
-        <v>6300</v>
+        <v>8000</v>
       </c>
       <c r="H711">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I711" t="inlineStr">
         <is>
@@ -27393,31 +27393,31 @@
     <row r="712">
       <c r="A712" t="inlineStr">
         <is>
-          <t>Bharat Heavy Electricals Limited</t>
+          <t>Mahrishi Alloys Pvt. Ltd.</t>
         </is>
       </c>
       <c r="B712" t="inlineStr">
         <is>
-          <t>Quartz Powder</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C712">
-        <v>223662.6</v>
+        <v>250607.5</v>
       </c>
       <c r="D712">
-        <v>11183.13</v>
+        <v>31988.98</v>
       </c>
       <c r="E712">
-        <v>234845</v>
+        <v>295716.9</v>
       </c>
       <c r="F712">
-        <v>51.23999999999999</v>
+        <v>77.11</v>
       </c>
       <c r="G712">
-        <v>4365.000000000001</v>
+        <v>3250</v>
       </c>
       <c r="H712">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I712" t="inlineStr">
         <is>
@@ -27431,7 +27431,7 @@
     <row r="713">
       <c r="A713" t="inlineStr">
         <is>
-          <t>Mahrishi Alloys Pvt. Ltd.</t>
+          <t>Shivam Ispat (P) Ltd</t>
         </is>
       </c>
       <c r="B713" t="inlineStr">
@@ -27440,26 +27440,26 @@
         </is>
       </c>
       <c r="C713">
-        <v>166432.5</v>
+        <v>488329.5</v>
       </c>
       <c r="D713">
-        <v>31988.98</v>
+        <v>87899.31</v>
       </c>
       <c r="E713">
-        <v>196390.4</v>
+        <v>576228</v>
       </c>
       <c r="F713">
-        <v>51.20999999999999</v>
+        <v>75.70999999999999</v>
       </c>
       <c r="G713">
-        <v>3250</v>
+        <v>6450.000000000001</v>
       </c>
       <c r="H713">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I713" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Sunil Rathi</t>
         </is>
       </c>
       <c r="J713" s="2">
@@ -27469,35 +27469,35 @@
     <row r="714">
       <c r="A714" t="inlineStr">
         <is>
-          <t>Shri Tirupati Steel Cast Ltd</t>
+          <t>Pushpit Steels Private Limited</t>
         </is>
       </c>
       <c r="B714" t="inlineStr">
         <is>
-          <t>Nali Top</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C714">
-        <v>145152</v>
+        <v>439890</v>
       </c>
       <c r="D714">
-        <v>26127.36</v>
+        <v>39629.16</v>
       </c>
       <c r="E714">
-        <v>171278</v>
+        <v>519070.04</v>
       </c>
       <c r="F714">
-        <v>45.36</v>
+        <v>70.94999999999999</v>
       </c>
       <c r="G714">
-        <v>3200</v>
+        <v>6200.000000000001</v>
       </c>
       <c r="H714">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I714" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Abhijit Maloo</t>
         </is>
       </c>
       <c r="J714" s="2">
@@ -27507,28 +27507,28 @@
     <row r="715">
       <c r="A715" t="inlineStr">
         <is>
-          <t>PURVA STEEL PRIVATE LIMITED</t>
+          <t>Bharat Heavy Electricals Limited</t>
         </is>
       </c>
       <c r="B715" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Quartz Powder</t>
         </is>
       </c>
       <c r="C715">
-        <v>289024</v>
+        <v>223662.6</v>
       </c>
       <c r="D715">
-        <v>52024.32</v>
+        <v>11183.13</v>
       </c>
       <c r="E715">
-        <v>341048</v>
+        <v>234845</v>
       </c>
       <c r="F715">
-        <v>45.16</v>
+        <v>51.23999999999999</v>
       </c>
       <c r="G715">
-        <v>6400.000000000001</v>
+        <v>4365.000000000001</v>
       </c>
       <c r="H715">
         <v>2</v>
@@ -27545,35 +27545,35 @@
     <row r="716">
       <c r="A716" t="inlineStr">
         <is>
-          <t>Prime Gold International Limited</t>
+          <t>ILC IRON &amp; STEEL PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="B716" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C716">
-        <v>324880</v>
+        <v>298717</v>
       </c>
       <c r="D716">
-        <v>58478.4</v>
+        <v>0</v>
       </c>
       <c r="E716">
-        <v>383358</v>
+        <v>352486.06</v>
       </c>
       <c r="F716">
-        <v>40.61</v>
+        <v>48.97</v>
       </c>
       <c r="G716">
-        <v>8000</v>
+        <v>6100</v>
       </c>
       <c r="H716">
         <v>2</v>
       </c>
       <c r="I716" t="inlineStr">
         <is>
-          <t>Sharad Bhutra</t>
+          <t>Shresth Maheshwari</t>
         </is>
       </c>
       <c r="J716" s="2">
@@ -27583,35 +27583,35 @@
     <row r="717">
       <c r="A717" t="inlineStr">
         <is>
-          <t>MOHIT STEEL INDUSTRIES PVT LTD</t>
+          <t>Shri Tirupati Steel Cast Ltd</t>
         </is>
       </c>
       <c r="B717" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C717">
-        <v>258258</v>
+        <v>145152</v>
       </c>
       <c r="D717">
-        <v>46486.44</v>
+        <v>26127.36</v>
       </c>
       <c r="E717">
-        <v>304745</v>
+        <v>171278</v>
       </c>
       <c r="F717">
-        <v>40.04</v>
+        <v>45.36</v>
       </c>
       <c r="G717">
-        <v>6450</v>
+        <v>3200</v>
       </c>
       <c r="H717">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I717" t="inlineStr">
         <is>
-          <t>Sunil Rathi</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J717" s="2">
@@ -27621,31 +27621,31 @@
     <row r="718">
       <c r="A718" t="inlineStr">
         <is>
-          <t>Mahrishi Alloys Pvt. Ltd.</t>
+          <t>PURVA STEEL PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="B718" t="inlineStr">
         <is>
-          <t>Nali Top</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C718">
-        <v>61349</v>
+        <v>289024</v>
       </c>
       <c r="D718">
-        <v>9011.720000000001</v>
+        <v>52024.32</v>
       </c>
       <c r="E718">
-        <v>72392.12</v>
+        <v>341048</v>
       </c>
       <c r="F718">
-        <v>39.58</v>
+        <v>45.16</v>
       </c>
       <c r="G718">
-        <v>1550</v>
+        <v>6400.000000000001</v>
       </c>
       <c r="H718">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I718" t="inlineStr">
         <is>
@@ -27659,35 +27659,35 @@
     <row r="719">
       <c r="A719" t="inlineStr">
         <is>
-          <t>Sri Navdurga Billets Pvt Ltd</t>
+          <t>A One Steel &amp; Alloys Pvt Ltd.</t>
         </is>
       </c>
       <c r="B719" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C719">
-        <v>259442</v>
+        <v>323485.5</v>
       </c>
       <c r="D719">
-        <v>46699.56</v>
+        <v>0</v>
       </c>
       <c r="E719">
-        <v>306142</v>
+        <v>381712.89</v>
       </c>
       <c r="F719">
-        <v>35.54</v>
+        <v>40.69</v>
       </c>
       <c r="G719">
-        <v>7300</v>
+        <v>7950</v>
       </c>
       <c r="H719">
         <v>1</v>
       </c>
       <c r="I719" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Shresth Maheshwari</t>
         </is>
       </c>
       <c r="J719" s="2">
@@ -27697,35 +27697,35 @@
     <row r="720">
       <c r="A720" t="inlineStr">
         <is>
-          <t>Pushpit Steels Private Limited</t>
+          <t>Prime Gold International Limited</t>
         </is>
       </c>
       <c r="B720" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C720">
-        <v>220162</v>
+        <v>324880</v>
       </c>
       <c r="D720">
-        <v>39629.16</v>
+        <v>58478.4</v>
       </c>
       <c r="E720">
-        <v>259791</v>
+        <v>383358</v>
       </c>
       <c r="F720">
-        <v>35.51</v>
+        <v>40.61</v>
       </c>
       <c r="G720">
-        <v>6200</v>
+        <v>8000</v>
       </c>
       <c r="H720">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I720" t="inlineStr">
         <is>
-          <t>Abhijit Maloo</t>
+          <t>Sharad Bhutra</t>
         </is>
       </c>
       <c r="J720" s="2">
@@ -27735,7 +27735,7 @@
     <row r="721">
       <c r="A721" t="inlineStr">
         <is>
-          <t>MANDOVI CASTING PVT LTD</t>
+          <t>MOHIT STEEL INDUSTRIES PVT LTD</t>
         </is>
       </c>
       <c r="B721" t="inlineStr">
@@ -27744,16 +27744,16 @@
         </is>
       </c>
       <c r="C721">
-        <v>226395</v>
+        <v>258258</v>
       </c>
       <c r="D721">
-        <v>40751.1</v>
+        <v>46486.44</v>
       </c>
       <c r="E721">
-        <v>267146.1</v>
+        <v>304745</v>
       </c>
       <c r="F721">
-        <v>35.1</v>
+        <v>40.04</v>
       </c>
       <c r="G721">
         <v>6450</v>
@@ -27773,35 +27773,35 @@
     <row r="722">
       <c r="A722" t="inlineStr">
         <is>
-          <t>Pattambi Brothers</t>
+          <t>Mahrishi Alloys Pvt. Ltd.</t>
         </is>
       </c>
       <c r="B722" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C722">
-        <v>220941</v>
+        <v>61349</v>
       </c>
       <c r="D722">
-        <v>39769.38</v>
+        <v>9011.720000000001</v>
       </c>
       <c r="E722">
-        <v>260710.38</v>
+        <v>72392.12</v>
       </c>
       <c r="F722">
-        <v>35.07</v>
+        <v>39.58</v>
       </c>
       <c r="G722">
-        <v>6300</v>
+        <v>1550</v>
       </c>
       <c r="H722">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I722" t="inlineStr">
         <is>
-          <t>Vishnu Kankani</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J722" s="2">
@@ -27811,35 +27811,35 @@
     <row r="723">
       <c r="A723" t="inlineStr">
         <is>
-          <t>JEPPIAAR FURNACE AND STEELS PVT.LTD</t>
+          <t>A One Steels And Alloys Pvt Ltd</t>
         </is>
       </c>
       <c r="B723" t="inlineStr">
         <is>
-          <t>Boron Oxide Premix</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C723">
-        <v>319792</v>
+        <v>138472</v>
       </c>
       <c r="D723">
-        <v>57562.56</v>
+        <v>0</v>
       </c>
       <c r="E723">
-        <v>377355</v>
+        <v>163396.96</v>
       </c>
       <c r="F723">
-        <v>34.76000000000001</v>
+        <v>36.44</v>
       </c>
       <c r="G723">
-        <v>9199.999999999998</v>
+        <v>3800</v>
       </c>
       <c r="H723">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I723" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Shresth Maheshwari</t>
         </is>
       </c>
       <c r="J723" s="2">
@@ -27849,35 +27849,35 @@
     <row r="724">
       <c r="A724" t="inlineStr">
         <is>
-          <t>Sugna Sponge &amp; Power Pvt Ltd</t>
+          <t>Prakash Sponge Iron &amp; Power Pvt Ltd</t>
         </is>
       </c>
       <c r="B724" t="inlineStr">
         <is>
-          <t>Nali Top</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C724">
-        <v>128353</v>
+        <v>269344</v>
       </c>
       <c r="D724">
-        <v>23103.54</v>
+        <v>0</v>
       </c>
       <c r="E724">
-        <v>151457</v>
+        <v>317825.92</v>
       </c>
       <c r="F724">
-        <v>34.69</v>
+        <v>35.44</v>
       </c>
       <c r="G724">
-        <v>3700</v>
+        <v>7600.000000000001</v>
       </c>
       <c r="H724">
         <v>1</v>
       </c>
       <c r="I724" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Shresth Maheshwari</t>
         </is>
       </c>
       <c r="J724" s="2">
@@ -27887,35 +27887,35 @@
     <row r="725">
       <c r="A725" t="inlineStr">
         <is>
-          <t>A One Steels And Alloys Pvt Ltd</t>
+          <t>MINAR ISPAT PVT. LTD</t>
         </is>
       </c>
       <c r="B725" t="inlineStr">
         <is>
-          <t>Nali Top</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C725">
-        <v>124450</v>
+        <v>210570.5</v>
       </c>
       <c r="D725">
-        <v>22401</v>
+        <v>0</v>
       </c>
       <c r="E725">
-        <v>146851</v>
+        <v>248473.19</v>
       </c>
       <c r="F725">
-        <v>32.75</v>
+        <v>35.39</v>
       </c>
       <c r="G725">
-        <v>3800</v>
+        <v>5950</v>
       </c>
       <c r="H725">
         <v>1</v>
       </c>
       <c r="I725" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Abhijit Maloo</t>
         </is>
       </c>
       <c r="J725" s="2">
@@ -27925,35 +27925,35 @@
     <row r="726">
       <c r="A726" t="inlineStr">
         <is>
-          <t>Sri Vinayaga Alloys (P) Ltd</t>
+          <t>SHRADDHA ISPAT-MELTING DIVISION</t>
         </is>
       </c>
       <c r="B726" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C726">
-        <v>195930</v>
+        <v>119816</v>
       </c>
       <c r="D726">
-        <v>35267.4</v>
+        <v>0</v>
       </c>
       <c r="E726">
-        <v>231197</v>
+        <v>141382.88</v>
       </c>
       <c r="F726">
-        <v>31.1</v>
+        <v>35.23999999999999</v>
       </c>
       <c r="G726">
-        <v>6300</v>
+        <v>3400</v>
       </c>
       <c r="H726">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I726" t="inlineStr">
         <is>
-          <t>Vishnu Kankani</t>
+          <t>Sunil Rathi</t>
         </is>
       </c>
       <c r="J726" s="2">
@@ -27963,7 +27963,7 @@
     <row r="727">
       <c r="A727" t="inlineStr">
         <is>
-          <t>GOVAAN STEELS PRIVATE LIMITED</t>
+          <t>MANDOVI CASTING PVT LTD</t>
         </is>
       </c>
       <c r="B727" t="inlineStr">
@@ -27972,26 +27972,26 @@
         </is>
       </c>
       <c r="C727">
-        <v>193408</v>
+        <v>226395</v>
       </c>
       <c r="D727">
-        <v>34813.44</v>
+        <v>40751.1</v>
       </c>
       <c r="E727">
-        <v>228221</v>
+        <v>267146.1</v>
       </c>
       <c r="F727">
-        <v>30.22</v>
+        <v>35.1</v>
       </c>
       <c r="G727">
-        <v>6400</v>
+        <v>6450</v>
       </c>
       <c r="H727">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I727" t="inlineStr">
         <is>
-          <t>Vishnu Kankani</t>
+          <t>Sunil Rathi</t>
         </is>
       </c>
       <c r="J727" s="2">
@@ -28001,7 +28001,7 @@
     <row r="728">
       <c r="A728" t="inlineStr">
         <is>
-          <t>M.A.STEELS (P) LTD</t>
+          <t>Pattambi Brothers</t>
         </is>
       </c>
       <c r="B728" t="inlineStr">
@@ -28010,16 +28010,16 @@
         </is>
       </c>
       <c r="C728">
-        <v>189063</v>
+        <v>220941</v>
       </c>
       <c r="D728">
-        <v>34031.34</v>
+        <v>39769.38</v>
       </c>
       <c r="E728">
-        <v>223094</v>
+        <v>260710.38</v>
       </c>
       <c r="F728">
-        <v>30.01</v>
+        <v>35.07</v>
       </c>
       <c r="G728">
         <v>6300</v>
@@ -28039,31 +28039,31 @@
     <row r="729">
       <c r="A729" t="inlineStr">
         <is>
-          <t>ARDEX ENDURA (INDIA) PRIVATE LIMITED Quartztech</t>
+          <t>JEPPIAAR FURNACE AND STEELS PVT.LTD</t>
         </is>
       </c>
       <c r="B729" t="inlineStr">
         <is>
-          <t>Quartz Powder</t>
+          <t>Boron Oxide Premix</t>
         </is>
       </c>
       <c r="C729">
-        <v>80620.8</v>
+        <v>319792</v>
       </c>
       <c r="D729">
-        <v>4031.04</v>
+        <v>57562.56</v>
       </c>
       <c r="E729">
-        <v>84652</v>
+        <v>377355</v>
       </c>
       <c r="F729">
-        <v>29.64</v>
+        <v>34.76000000000001</v>
       </c>
       <c r="G729">
-        <v>2720</v>
+        <v>9199.999999999998</v>
       </c>
       <c r="H729">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I729" t="inlineStr">
         <is>
@@ -28077,31 +28077,31 @@
     <row r="730">
       <c r="A730" t="inlineStr">
         <is>
-          <t>Ardex Endura (India) Private Ltd</t>
+          <t>Sugna Sponge &amp; Power Pvt Ltd</t>
         </is>
       </c>
       <c r="B730" t="inlineStr">
         <is>
-          <t>Quartz Powder</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C730">
-        <v>109200</v>
+        <v>128353</v>
       </c>
       <c r="D730">
-        <v>5460</v>
+        <v>23103.54</v>
       </c>
       <c r="E730">
-        <v>114660</v>
+        <v>151457</v>
       </c>
       <c r="F730">
-        <v>27.3</v>
+        <v>34.69</v>
       </c>
       <c r="G730">
-        <v>4000</v>
+        <v>3700</v>
       </c>
       <c r="H730">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I730" t="inlineStr">
         <is>
@@ -28115,35 +28115,35 @@
     <row r="731">
       <c r="A731" t="inlineStr">
         <is>
-          <t>ILC IRON &amp; STEEL PRIVATE LIMITED</t>
+          <t>A One Steels And Alloys Pvt Ltd</t>
         </is>
       </c>
       <c r="B731" t="inlineStr">
         <is>
-          <t>Boric Acid Premix</t>
+          <t>Nali Top</t>
         </is>
       </c>
       <c r="C731">
-        <v>124745</v>
+        <v>124450</v>
       </c>
       <c r="D731">
-        <v>0</v>
+        <v>22401</v>
       </c>
       <c r="E731">
-        <v>147199.1</v>
+        <v>146851</v>
       </c>
       <c r="F731">
-        <v>20.45</v>
+        <v>32.75</v>
       </c>
       <c r="G731">
-        <v>6100</v>
+        <v>3800</v>
       </c>
       <c r="H731">
         <v>1</v>
       </c>
       <c r="I731" t="inlineStr">
         <is>
-          <t>Shresth Maheshwari</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="J731" s="2">
@@ -28153,35 +28153,35 @@
     <row r="732">
       <c r="A732" t="inlineStr">
         <is>
-          <t>Adishakti Smelters Private Limited</t>
+          <t>Sri Vinayaga Alloys (P) Ltd</t>
         </is>
       </c>
       <c r="B732" t="inlineStr">
         <is>
-          <t>Nali Top</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C732">
-        <v>28432</v>
+        <v>195930</v>
       </c>
       <c r="D732">
-        <v>0</v>
+        <v>35267.4</v>
       </c>
       <c r="E732">
-        <v>33549.75999999999</v>
+        <v>231197</v>
       </c>
       <c r="F732">
-        <v>17.77</v>
+        <v>31.1</v>
       </c>
       <c r="G732">
-        <v>1600</v>
+        <v>6300</v>
       </c>
       <c r="H732">
         <v>2</v>
       </c>
       <c r="I732" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Vishnu Kankani</t>
         </is>
       </c>
       <c r="J732" s="2">
@@ -28191,35 +28191,35 @@
     <row r="733">
       <c r="A733" t="inlineStr">
         <is>
-          <t>ILC IRON &amp; STEEL PRIVATE LIMITED</t>
+          <t>GOVAAN STEELS PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="B733" t="inlineStr">
         <is>
-          <t>Nali Top</t>
+          <t>Boric Acid Premix</t>
         </is>
       </c>
       <c r="C733">
-        <v>29970</v>
+        <v>193408</v>
       </c>
       <c r="D733">
-        <v>27848.7</v>
+        <v>34813.44</v>
       </c>
       <c r="E733">
-        <v>35364.6</v>
+        <v>228221</v>
       </c>
       <c r="F733">
-        <v>9.99</v>
+        <v>30.22</v>
       </c>
       <c r="G733">
-        <v>3000</v>
+        <v>6400</v>
       </c>
       <c r="H733">
         <v>1</v>
       </c>
       <c r="I733" t="inlineStr">
         <is>
-          <t>Shresth Maheshwari</t>
+          <t>Vishnu Kankani</t>
         </is>
       </c>
       <c r="J733" s="2">
@@ -28229,38 +28229,266 @@
     <row r="734">
       <c r="A734" t="inlineStr">
         <is>
+          <t>M.A.STEELS (P) LTD</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Boric Acid Premix</t>
+        </is>
+      </c>
+      <c r="C734">
+        <v>189063</v>
+      </c>
+      <c r="D734">
+        <v>34031.34</v>
+      </c>
+      <c r="E734">
+        <v>223094</v>
+      </c>
+      <c r="F734">
+        <v>30.01</v>
+      </c>
+      <c r="G734">
+        <v>6300</v>
+      </c>
+      <c r="H734">
+        <v>1</v>
+      </c>
+      <c r="I734" t="inlineStr">
+        <is>
+          <t>Vishnu Kankani</t>
+        </is>
+      </c>
+      <c r="J734" s="2">
+        <v>45108</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>PREMIUM FERRO ALLOYS LIMITED</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Boric Acid Premix</t>
+        </is>
+      </c>
+      <c r="C735">
+        <v>188244</v>
+      </c>
+      <c r="D735">
+        <v>0</v>
+      </c>
+      <c r="E735">
+        <v>222127.92</v>
+      </c>
+      <c r="F735">
+        <v>29.88</v>
+      </c>
+      <c r="G735">
+        <v>6300</v>
+      </c>
+      <c r="H735">
+        <v>1</v>
+      </c>
+      <c r="I735" t="inlineStr">
+        <is>
+          <t>Shresth Maheshwari</t>
+        </is>
+      </c>
+      <c r="J735" s="2">
+        <v>45108</v>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>ARDEX ENDURA (INDIA) PRIVATE LIMITED Quartztech</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Quartz Powder</t>
+        </is>
+      </c>
+      <c r="C736">
+        <v>80620.8</v>
+      </c>
+      <c r="D736">
+        <v>4031.04</v>
+      </c>
+      <c r="E736">
+        <v>84652</v>
+      </c>
+      <c r="F736">
+        <v>29.64</v>
+      </c>
+      <c r="G736">
+        <v>2720</v>
+      </c>
+      <c r="H736">
+        <v>1</v>
+      </c>
+      <c r="I736" t="inlineStr">
+        <is>
+          <t>Direct</t>
+        </is>
+      </c>
+      <c r="J736" s="2">
+        <v>45108</v>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>Ardex Endura (India) Private Ltd</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Quartz Powder</t>
+        </is>
+      </c>
+      <c r="C737">
+        <v>109200</v>
+      </c>
+      <c r="D737">
+        <v>5460</v>
+      </c>
+      <c r="E737">
+        <v>114660</v>
+      </c>
+      <c r="F737">
+        <v>27.3</v>
+      </c>
+      <c r="G737">
+        <v>4000</v>
+      </c>
+      <c r="H737">
+        <v>2</v>
+      </c>
+      <c r="I737" t="inlineStr">
+        <is>
+          <t>Direct</t>
+        </is>
+      </c>
+      <c r="J737" s="2">
+        <v>45108</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>Adishakti Smelters Private Limited</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Nali Top</t>
+        </is>
+      </c>
+      <c r="C738">
+        <v>28432</v>
+      </c>
+      <c r="D738">
+        <v>0</v>
+      </c>
+      <c r="E738">
+        <v>33549.75999999999</v>
+      </c>
+      <c r="F738">
+        <v>17.77</v>
+      </c>
+      <c r="G738">
+        <v>1600</v>
+      </c>
+      <c r="H738">
+        <v>2</v>
+      </c>
+      <c r="I738" t="inlineStr">
+        <is>
+          <t>Direct</t>
+        </is>
+      </c>
+      <c r="J738" s="2">
+        <v>45108</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>ILC IRON &amp; STEEL PRIVATE LIMITED</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Nali Top</t>
+        </is>
+      </c>
+      <c r="C739">
+        <v>49020</v>
+      </c>
+      <c r="D739">
+        <v>27848.7</v>
+      </c>
+      <c r="E739">
+        <v>57843.6</v>
+      </c>
+      <c r="F739">
+        <v>16.34</v>
+      </c>
+      <c r="G739">
+        <v>3000</v>
+      </c>
+      <c r="H739">
+        <v>2</v>
+      </c>
+      <c r="I739" t="inlineStr">
+        <is>
+          <t>Shresth Maheshwari</t>
+        </is>
+      </c>
+      <c r="J739" s="2">
+        <v>45108</v>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
           <t>Oswal Smelters Pvt Ltd</t>
         </is>
       </c>
-      <c r="B734" t="inlineStr">
+      <c r="B740" t="inlineStr">
         <is>
           <t>Quartz Grain</t>
         </is>
       </c>
-      <c r="C734">
-        <v>11772.5</v>
-      </c>
-      <c r="D734">
+      <c r="C740">
+        <v>21802.5</v>
+      </c>
+      <c r="D740">
         <v>588.62</v>
       </c>
-      <c r="E734">
-        <v>12361</v>
-      </c>
-      <c r="F734">
-        <v>2.77</v>
-      </c>
-      <c r="G734">
+      <c r="E740">
+        <v>22892.5</v>
+      </c>
+      <c r="F740">
+        <v>5.13</v>
+      </c>
+      <c r="G740">
         <v>4250</v>
       </c>
-      <c r="H734">
-        <v>1</v>
-      </c>
-      <c r="I734" t="inlineStr">
-        <is>
-          <t>Direct</t>
-        </is>
-      </c>
-      <c r="J734" s="2">
+      <c r="H740">
+        <v>2</v>
+      </c>
+      <c r="I740" t="inlineStr">
+        <is>
+          <t>Direct</t>
+        </is>
+      </c>
+      <c r="J740" s="2">
         <v>45108</v>
       </c>
     </row>

</xml_diff>